<commit_message>
asset page : show storage map, fix save file bug
</commit_message>
<xml_diff>
--- a/data/db/data providers.xlsx
+++ b/data/db/data providers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD34690-4989-4E7B-925C-A79DA84F4A7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082617F9-86FA-4CB1-B59F-23B7EAF37C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$92</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="132">
   <si>
     <t>Amazon</t>
   </si>
@@ -165,45 +168,24 @@
     <t>NORTHAMERICA-NORTHEAST1</t>
   </si>
   <si>
-    <t>Montréal</t>
-  </si>
-  <si>
     <t>US-CENTRAL1</t>
   </si>
   <si>
-    <t>Iowa</t>
-  </si>
-  <si>
     <t>US-EAST1</t>
   </si>
   <si>
-    <t>Caroline du Sud</t>
-  </si>
-  <si>
     <t>US-EAST4</t>
   </si>
   <si>
-    <t>Virginie du Nord</t>
-  </si>
-  <si>
     <t>US-WEST1</t>
   </si>
   <si>
-    <t>Oregon</t>
-  </si>
-  <si>
     <t>US-WEST2</t>
   </si>
   <si>
-    <t>Los Angeles</t>
-  </si>
-  <si>
     <t>SOUTHAMERICA-EAST1</t>
   </si>
   <si>
-    <t>São Paulo</t>
-  </si>
-  <si>
     <t>EUROPE-NORTH1</t>
   </si>
   <si>
@@ -219,15 +201,9 @@
     <t>EUROPE-WEST2</t>
   </si>
   <si>
-    <t>Londres</t>
-  </si>
-  <si>
     <t>EUROPE-WEST3</t>
   </si>
   <si>
-    <t>Francfort</t>
-  </si>
-  <si>
     <t>EUROPE-WEST4</t>
   </si>
   <si>
@@ -237,9 +213,6 @@
     <t>EUROPE-WEST6</t>
   </si>
   <si>
-    <t>Zurich</t>
-  </si>
-  <si>
     <t>ASIA-EAST1</t>
   </si>
   <si>
@@ -252,21 +225,12 @@
     <t>ASIA-NORTHEAST1</t>
   </si>
   <si>
-    <t>Tokyo</t>
-  </si>
-  <si>
     <t>ASIA-NORTHEAST2</t>
   </si>
   <si>
-    <t>Osaka</t>
-  </si>
-  <si>
     <t>ASIA-SOUTH1</t>
   </si>
   <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
     <t>ASIA-SOUTHEAST1</t>
   </si>
   <si>
@@ -276,9 +240,6 @@
     <t>AUSTRALIA-SOUTHEAST1</t>
   </si>
   <si>
-    <t>Sydney</t>
-  </si>
-  <si>
     <t>Google</t>
   </si>
   <si>
@@ -466,6 +427,12 @@
   </si>
   <si>
     <t>data provider</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
   </si>
 </sst>
 </file>
@@ -499,7 +466,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -509,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -562,6 +535,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC19A3D-01C7-400F-ABF6-368E3B90A145}">
-  <dimension ref="A1:H92"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -892,9 +866,9 @@
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -911,8 +885,14 @@
       <c r="F1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="G1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -931,12 +911,18 @@
       <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE("(",B2,",",C2,",'",D2,"','",E2,"','",F2,"'),")</f>
-        <v>(1,1,'US East (Ohio)','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="G2" s="6">
+        <v>-82.9</v>
+      </c>
+      <c r="H2" s="6">
+        <v>39.9</v>
+      </c>
+      <c r="J2" t="str">
+        <f>CONCATENATE("(",B2,",",C2,",'",D2,"','",E2,"','",F2,"','",G2,"','",H2,"'),")</f>
+        <v>(1,1,'US East (Ohio)','Amérique du Nord','Etats-Unis','-82.9','39.9'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -955,12 +941,18 @@
       <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H66" si="0">CONCATENATE("(",B3,",",C3,",'",D3,"','",E3,"','",F3,"'),")</f>
-        <v>(2,1,'US East (N. Virginia)','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="G3" s="6">
+        <v>-77.400000000000006</v>
+      </c>
+      <c r="H3" s="6">
+        <v>37.5</v>
+      </c>
+      <c r="J3" t="str">
+        <f t="shared" ref="J3:J66" si="0">CONCATENATE("(",B3,",",C3,",'",D3,"','",E3,"','",F3,"','",G3,"','",H3,"'),")</f>
+        <v>(2,1,'US East (N. Virginia)','Amérique du Nord','Etats-Unis','-77.4','37.5'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -979,12 +971,18 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="str">
+      <c r="G4" s="6">
+        <v>-121.5</v>
+      </c>
+      <c r="H4" s="6">
+        <v>38.6</v>
+      </c>
+      <c r="J4" t="str">
         <f t="shared" si="0"/>
-        <v>(3,1,'US West (N. California)','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>(3,1,'US West (N. California)','Amérique du Nord','Etats-Unis','-121.5','38.6'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1003,12 +1001,18 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="str">
+      <c r="G5" s="6">
+        <v>-122.7</v>
+      </c>
+      <c r="H5" s="6">
+        <v>45.5</v>
+      </c>
+      <c r="J5" t="str">
         <f t="shared" si="0"/>
-        <v>(4,1,'US West (Oregon)','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>(4,1,'US West (Oregon)','Amérique du Nord','Etats-Unis','-122.7','45.5'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1027,12 +1031,20 @@
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>(5,1,'Asia Pacific (Hong Kong)','Asie-Pacifique','Hong Kong'),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="G6">
+        <f ca="1">RANDBETWEEN(-180,180)</f>
+        <v>62</v>
+      </c>
+      <c r="H6">
+        <f ca="1">RANDBETWEEN(-50,50)</f>
+        <v>14</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(5,1,'Asia Pacific (Hong Kong)','Asie-Pacifique','Hong Kong','62','14'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1051,12 +1063,20 @@
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>(6,1,'Asia Pacific (Mumbai)','Asie-Pacifique','Inde'),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="G7">
+        <f t="shared" ref="G7:G70" ca="1" si="1">RANDBETWEEN(-180,180)</f>
+        <v>41</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H70" ca="1" si="2">RANDBETWEEN(-50,50)</f>
+        <v>4</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(6,1,'Asia Pacific (Mumbai)','Asie-Pacifique','Inde','41','4'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1075,12 +1095,20 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>(7,1,'Asia Pacific (Osaka-Local)','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="G8">
+        <f t="shared" ca="1" si="1"/>
+        <v>-70</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(7,1,'Asia Pacific (Osaka-Local)','Asie-Pacifique','Japon','-70','34'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1099,12 +1127,20 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>(8,1,'Asia Pacific (Seoul)','Asie-Pacifique','Corée du Sud'),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="G9">
+        <f t="shared" ca="1" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(8,1,'Asia Pacific (Seoul)','Asie-Pacifique','Corée du Sud','162','47'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1121,14 +1157,22 @@
         <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>(9,1,'Asia Pacific (Singapore)','Asie-Pacifique','Singapour'),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>65</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="1"/>
+        <v>-49</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="2"/>
+        <v>-13</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(9,1,'Asia Pacific (Singapore)','Asie-Pacifique','Singapour','-49','-13'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1147,12 +1191,20 @@
       <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>(10,1,'Asia Pacific (Sydney)','Asie-Pacifique','Australie'),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="G11">
+        <f t="shared" ca="1" si="1"/>
+        <v>-71</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(10,1,'Asia Pacific (Sydney)','Asie-Pacifique','Australie','-71','25'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1171,12 +1223,20 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>(11,1,'Asia Pacific (Tokyo)','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="G12">
+        <f t="shared" ca="1" si="1"/>
+        <v>-158</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(11,1,'Asia Pacific (Tokyo)','Asie-Pacifique','Japon','-158','3'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1195,12 +1255,20 @@
       <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>(12,1,'Canada (Central)','Amérique du Nord','Canada'),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="G13">
+        <f t="shared" ca="1" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="2"/>
+        <v>-24</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(12,1,'Canada (Central)','Amérique du Nord','Canada','163','-24'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1219,12 +1287,20 @@
       <c r="F14" t="s">
         <v>37</v>
       </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>(13,1,'Europe (Frankfurt)','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="G14">
+        <f t="shared" ca="1" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(13,1,'Europe (Frankfurt)','Europe','Allemagne','128','14'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1243,12 +1319,20 @@
       <c r="F15" t="s">
         <v>38</v>
       </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>(14,1,'Europe (Ireland)','Europe','Irlande'),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="G15">
+        <f t="shared" ca="1" si="1"/>
+        <v>-46</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(14,1,'Europe (Ireland)','Europe','Irlande','-46','27'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1267,12 +1351,20 @@
       <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>(15,1,'Europe (London)','Europe','Grande-Bretagne'),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="G16">
+        <f t="shared" ca="1" si="1"/>
+        <v>66</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="J16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(15,1,'Europe (London)','Europe','Grande-Bretagne','66','45'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1291,12 +1383,20 @@
       <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>(16,1,'Europe (Paris)','Europe','France'),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="G17">
+        <f t="shared" ca="1" si="1"/>
+        <v>-179</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="J17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(16,1,'Europe (Paris)','Europe','France','-179','4'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1315,12 +1415,20 @@
       <c r="F18" t="s">
         <v>41</v>
       </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>(17,1,'Europe (Stockholm)','Europe','Suède'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="G18">
+        <f t="shared" ca="1" si="1"/>
+        <v>179</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="J18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(17,1,'Europe (Stockholm)','Europe','Suède','179','33'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1339,12 +1447,20 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>(18,1,'Middle East (Bahrain)','Asie-Pacifique','Bahrain'),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="G19">
+        <f t="shared" ca="1" si="1"/>
+        <v>-36</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(18,1,'Middle East (Bahrain)','Asie-Pacifique','Bahrain','-36','28'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1361,16 +1477,24 @@
         <v>29</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>(19,1,'South America (São Paulo)','Amérique du Sud','Brésil'),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="1"/>
+        <v>-25</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="J20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(19,1,'South America (São Paulo)','Amérique du Sud','Brésil','-25','46'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -1387,14 +1511,22 @@
       <c r="F21" t="s">
         <v>24</v>
       </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>(20,2,'NORTHAMERICA-NORTHEAST1','Amérique du Nord','Canada'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="G21">
+        <f t="shared" ca="1" si="1"/>
+        <v>62</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="J21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(20,2,'NORTHAMERICA-NORTHEAST1','Amérique du Nord','Canada','62','3'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -1403,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
@@ -1411,14 +1543,22 @@
       <c r="F22" t="s">
         <v>30</v>
       </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v>(21,2,'US-CENTRAL1','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="G22">
+        <f t="shared" ca="1" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="J22" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(21,2,'US-CENTRAL1','Amérique du Nord','Etats-Unis','46','29'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -1427,7 +1567,7 @@
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
         <v>27</v>
@@ -1435,14 +1575,22 @@
       <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>(22,2,'US-EAST1','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="G23">
+        <f t="shared" ca="1" si="1"/>
+        <v>-92</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="2"/>
+        <v>-43</v>
+      </c>
+      <c r="J23" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(22,2,'US-EAST1','Amérique du Nord','Etats-Unis','-92','-43'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -1451,7 +1599,7 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
         <v>27</v>
@@ -1459,14 +1607,22 @@
       <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v>(23,2,'US-EAST4','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="G24">
+        <f t="shared" ca="1" si="1"/>
+        <v>-160</v>
+      </c>
+      <c r="H24">
+        <f t="shared" ca="1" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="J24" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(23,2,'US-EAST4','Amérique du Nord','Etats-Unis','-160','11'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -1475,7 +1631,7 @@
         <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E25" t="s">
         <v>27</v>
@@ -1483,14 +1639,22 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v>(24,2,'US-WEST1','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="G25">
+        <f t="shared" ca="1" si="1"/>
+        <v>161</v>
+      </c>
+      <c r="H25">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(24,2,'US-WEST1','Amérique du Nord','Etats-Unis','161','0'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -1499,7 +1663,7 @@
         <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E26" t="s">
         <v>27</v>
@@ -1507,14 +1671,22 @@
       <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>(25,2,'US-WEST2','Amérique du Nord','Etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="G26">
+        <f t="shared" ca="1" si="1"/>
+        <v>83</v>
+      </c>
+      <c r="H26">
+        <f t="shared" ca="1" si="2"/>
+        <v>-25</v>
+      </c>
+      <c r="J26" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(25,2,'US-WEST2','Amérique du Nord','Etats-Unis','83','-25'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -1523,22 +1695,30 @@
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v>(26,2,'SOUTHAMERICA-EAST1','Amérique du Sud','Brésil'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="G27">
+        <f t="shared" ca="1" si="1"/>
+        <v>63</v>
+      </c>
+      <c r="H27">
+        <f t="shared" ca="1" si="2"/>
+        <v>-34</v>
+      </c>
+      <c r="J27" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(26,2,'SOUTHAMERICA-EAST1','Amérique du Sud','Brésil','63','-34'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -1547,22 +1727,30 @@
         <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="E28" t="s">
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>57</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v>(27,2,'EUROPE-NORTH1','Europe','Finlande'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+        <v>50</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ca="1" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="H28">
+        <f t="shared" ca="1" si="2"/>
+        <v>-22</v>
+      </c>
+      <c r="J28" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(27,2,'EUROPE-NORTH1','Europe','Finlande','95','-22'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -1571,22 +1759,30 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E29" t="s">
         <v>25</v>
       </c>
       <c r="F29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v>(28,2,'EUROPE-WEST1','Europe','Belgique'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>52</v>
+      </c>
+      <c r="G29">
+        <f t="shared" ca="1" si="1"/>
+        <v>143</v>
+      </c>
+      <c r="H29">
+        <f t="shared" ca="1" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="J29" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(28,2,'EUROPE-WEST1','Europe','Belgique','143','43'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -1595,7 +1791,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -1603,14 +1799,22 @@
       <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>(29,2,'EUROPE-WEST2','Europe','Grande-Bretagne'),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="G30">
+        <f t="shared" ca="1" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="H30">
+        <f t="shared" ca="1" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="J30" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(29,2,'EUROPE-WEST2','Europe','Grande-Bretagne','131','-16'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -1619,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E31" t="s">
         <v>25</v>
@@ -1627,14 +1831,22 @@
       <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>(30,2,'EUROPE-WEST3','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="G31">
+        <f t="shared" ca="1" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ca="1" si="2"/>
+        <v>-32</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(30,2,'EUROPE-WEST3','Europe','Allemagne','133','-32'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -1643,22 +1855,30 @@
         <v>2</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E32" t="s">
         <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>(31,2,'EUROPE-WEST4','Europe','Pays-Bas'),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8">
+        <v>56</v>
+      </c>
+      <c r="G32">
+        <f t="shared" ca="1" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="H32">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(31,2,'EUROPE-WEST4','Europe','Pays-Bas','116','34'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -1667,22 +1887,30 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E33" t="s">
         <v>25</v>
       </c>
       <c r="F33" t="s">
-        <v>83</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>(32,2,'EUROPE-WEST6','Europe','Suisse'),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>69</v>
+      </c>
+      <c r="G33">
+        <f t="shared" ca="1" si="1"/>
+        <v>-122</v>
+      </c>
+      <c r="H33">
+        <f t="shared" ca="1" si="2"/>
+        <v>-48</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(32,2,'EUROPE-WEST6','Europe','Suisse','-122','-48'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -1691,22 +1919,30 @@
         <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E34" t="s">
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" t="str">
-        <f t="shared" si="0"/>
-        <v>(33,2,'ASIA-EAST1','Asie-Pacifique','Taïwan'),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
+        <v>59</v>
+      </c>
+      <c r="G34">
+        <f t="shared" ca="1" si="1"/>
+        <v>-119</v>
+      </c>
+      <c r="H34">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(33,2,'ASIA-EAST1','Asie-Pacifique','Taïwan','-119','30'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -1715,7 +1951,7 @@
         <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E35" t="s">
         <v>28</v>
@@ -1723,14 +1959,22 @@
       <c r="F35" t="s">
         <v>31</v>
       </c>
-      <c r="H35" t="str">
-        <f t="shared" si="0"/>
-        <v>(34,2,'ASIA-EAST2','Asie-Pacifique','Hong Kong'),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="G35">
+        <f t="shared" ca="1" si="1"/>
+        <v>-53</v>
+      </c>
+      <c r="H35">
+        <f t="shared" ca="1" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(34,2,'ASIA-EAST2','Asie-Pacifique','Hong Kong','-53','31'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -1739,7 +1983,7 @@
         <v>2</v>
       </c>
       <c r="D36" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="E36" t="s">
         <v>28</v>
@@ -1747,14 +1991,22 @@
       <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="H36" t="str">
-        <f t="shared" si="0"/>
-        <v>(35,2,'ASIA-NORTHEAST1','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="G36">
+        <f t="shared" ca="1" si="1"/>
+        <v>177</v>
+      </c>
+      <c r="H36">
+        <f t="shared" ca="1" si="2"/>
+        <v>-17</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(35,2,'ASIA-NORTHEAST1','Asie-Pacifique','Japon','177','-17'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -1763,7 +2015,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E37" t="s">
         <v>28</v>
@@ -1771,14 +2023,22 @@
       <c r="F37" t="s">
         <v>34</v>
       </c>
-      <c r="H37" t="str">
-        <f t="shared" si="0"/>
-        <v>(36,2,'ASIA-NORTHEAST2','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="G37">
+        <f t="shared" ca="1" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="H37">
+        <f t="shared" ca="1" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="J37" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(36,2,'ASIA-NORTHEAST2','Asie-Pacifique','Japon','162','28'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -1787,7 +2047,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E38" t="s">
         <v>28</v>
@@ -1795,14 +2055,22 @@
       <c r="F38" t="s">
         <v>33</v>
       </c>
-      <c r="H38" t="str">
-        <f t="shared" si="0"/>
-        <v>(37,2,'ASIA-SOUTH1','Asie-Pacifique','Inde'),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="G38">
+        <f t="shared" ca="1" si="1"/>
+        <v>-39</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ca="1" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="J38" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(37,2,'ASIA-SOUTH1','Asie-Pacifique','Inde','-39','-10'),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -1811,22 +2079,30 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E39" t="s">
         <v>28</v>
       </c>
       <c r="F39" t="s">
-        <v>78</v>
-      </c>
-      <c r="H39" t="str">
-        <f t="shared" si="0"/>
-        <v>(38,2,'ASIA-SOUTHEAST1','Asie-Pacifique','Singapour'),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
+        <v>65</v>
+      </c>
+      <c r="G39">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="H39">
+        <f t="shared" ca="1" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="J39" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(38,2,'ASIA-SOUTHEAST1','Asie-Pacifique','Singapour','-100','-9'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -1835,7 +2111,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="E40" t="s">
         <v>28</v>
@@ -1843,14 +2119,22 @@
       <c r="F40" t="s">
         <v>36</v>
       </c>
-      <c r="H40" t="str">
-        <f t="shared" si="0"/>
-        <v>(39,2,'AUSTRALIA-SOUTHEAST1','Asie-Pacifique','Australie'),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="G40">
+        <f t="shared" ca="1" si="1"/>
+        <v>169</v>
+      </c>
+      <c r="H40">
+        <f t="shared" ca="1" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="J40" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(39,2,'AUSTRALIA-SOUTHEAST1','Asie-Pacifique','Australie','169','42'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -1859,7 +2143,7 @@
         <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="E41" t="s">
         <v>27</v>
@@ -1867,14 +2151,22 @@
       <c r="F41" t="s">
         <v>24</v>
       </c>
-      <c r="H41" t="str">
-        <f t="shared" si="0"/>
-        <v>(40,3,'Canada East','Amérique du Nord','Canada'),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="G41">
+        <f t="shared" ca="1" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="H41">
+        <f t="shared" ca="1" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="J41" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(40,3,'Canada East','Amérique du Nord','Canada','124','36'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -1883,7 +2175,7 @@
         <v>3</v>
       </c>
       <c r="D42" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E42" t="s">
         <v>27</v>
@@ -1891,14 +2183,22 @@
       <c r="F42" t="s">
         <v>24</v>
       </c>
-      <c r="H42" t="str">
-        <f t="shared" si="0"/>
-        <v>(41,3,'Canada Central','Amérique du Nord','Canada'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="G42">
+        <f t="shared" ca="1" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H42">
+        <f t="shared" ca="1" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="J42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(41,3,'Canada Central','Amérique du Nord','Canada','15','-16'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -1907,22 +2207,30 @@
         <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="E43" t="s">
         <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" t="str">
-        <f t="shared" si="0"/>
-        <v>(42,3,'US Gov Iowa','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G43">
+        <f t="shared" ca="1" si="1"/>
+        <v>-22</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ca="1" si="2"/>
+        <v>-13</v>
+      </c>
+      <c r="J43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(42,3,'US Gov Iowa','Amérique du Nord','etats-Unis','-22','-13'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -1931,22 +2239,30 @@
         <v>3</v>
       </c>
       <c r="D44" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="E44" t="s">
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>102</v>
-      </c>
-      <c r="H44" t="str">
-        <f t="shared" si="0"/>
-        <v>(43,3,'Central US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G44">
+        <f t="shared" ca="1" si="1"/>
+        <v>162</v>
+      </c>
+      <c r="H44">
+        <f t="shared" ca="1" si="2"/>
+        <v>-18</v>
+      </c>
+      <c r="J44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(43,3,'Central US','Amérique du Nord','etats-Unis','162','-18'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -1955,22 +2271,30 @@
         <v>3</v>
       </c>
       <c r="D45" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E45" t="s">
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>102</v>
-      </c>
-      <c r="H45" t="str">
-        <f t="shared" si="0"/>
-        <v>(44,3,'North Central US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G45">
+        <f t="shared" ca="1" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="H45">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(44,3,'North Central US','Amérique du Nord','etats-Unis','125','0'),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -1979,22 +2303,30 @@
         <v>3</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E46" t="s">
         <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
-      </c>
-      <c r="H46" t="str">
-        <f t="shared" si="0"/>
-        <v>(45,3,'US DoD East','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G46">
+        <f t="shared" ca="1" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="H46">
+        <f t="shared" ca="1" si="2"/>
+        <v>-36</v>
+      </c>
+      <c r="J46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(45,3,'US DoD East','Amérique du Nord','etats-Unis','69','-36'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -2003,22 +2335,30 @@
         <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
         <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
-      </c>
-      <c r="H47" t="str">
-        <f t="shared" si="0"/>
-        <v>(46,3,'East US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G47">
+        <f t="shared" ca="1" si="1"/>
+        <v>-143</v>
+      </c>
+      <c r="H47">
+        <f t="shared" ca="1" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="J47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(46,3,'East US','Amérique du Nord','etats-Unis','-143','30'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -2027,22 +2367,30 @@
         <v>3</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E48" t="s">
         <v>27</v>
       </c>
       <c r="F48" t="s">
-        <v>102</v>
-      </c>
-      <c r="H48" t="str">
-        <f t="shared" si="0"/>
-        <v>(47,3,'East US 2','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G48">
+        <f t="shared" ca="1" si="1"/>
+        <v>-96</v>
+      </c>
+      <c r="H48">
+        <f t="shared" ca="1" si="2"/>
+        <v>-38</v>
+      </c>
+      <c r="J48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(47,3,'East US 2','Amérique du Nord','etats-Unis','-96','-38'),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B49">
         <v>48</v>
@@ -2051,22 +2399,30 @@
         <v>3</v>
       </c>
       <c r="D49" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E49" t="s">
         <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
-      </c>
-      <c r="H49" t="str">
-        <f t="shared" si="0"/>
-        <v>(48,3,'US Gov Virginia','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G49">
+        <f t="shared" ca="1" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="H49">
+        <f t="shared" ca="1" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="J49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(48,3,'US Gov Virginia','Amérique du Nord','etats-Unis','-100','16'),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B50">
         <v>49</v>
@@ -2075,22 +2431,30 @@
         <v>3</v>
       </c>
       <c r="D50" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="E50" t="s">
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>102</v>
-      </c>
-      <c r="H50" t="str">
-        <f t="shared" si="0"/>
-        <v>(49,3,'US DoD Central','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G50">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H50">
+        <f t="shared" ca="1" si="2"/>
+        <v>-25</v>
+      </c>
+      <c r="J50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(49,3,'US DoD Central','Amérique du Nord','etats-Unis','40','-25'),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B51">
         <v>50</v>
@@ -2099,22 +2463,30 @@
         <v>3</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="E51" t="s">
         <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>102</v>
-      </c>
-      <c r="H51" t="str">
-        <f t="shared" si="0"/>
-        <v>(50,3,'West US 2','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G51">
+        <f t="shared" ca="1" si="1"/>
+        <v>-33</v>
+      </c>
+      <c r="H51">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="J51" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(50,3,'West US 2','Amérique du Nord','etats-Unis','-33','19'),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B52">
         <v>51</v>
@@ -2123,22 +2495,30 @@
         <v>3</v>
       </c>
       <c r="D52" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
         <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>102</v>
-      </c>
-      <c r="H52" t="str">
-        <f t="shared" si="0"/>
-        <v>(51,3,'West Central US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G52">
+        <f t="shared" ca="1" si="1"/>
+        <v>-84</v>
+      </c>
+      <c r="H52">
+        <f t="shared" ca="1" si="2"/>
+        <v>-33</v>
+      </c>
+      <c r="J52" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(51,3,'West Central US','Amérique du Nord','etats-Unis','-84','-33'),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B53">
         <v>52</v>
@@ -2147,22 +2527,30 @@
         <v>3</v>
       </c>
       <c r="D53" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="E53" t="s">
         <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
-      </c>
-      <c r="H53" t="str">
-        <f t="shared" si="0"/>
-        <v>(52,3,'West US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G53">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H53">
+        <f t="shared" ca="1" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="J53" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(52,3,'West US','Amérique du Nord','etats-Unis','8','-50'),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B54">
         <v>53</v>
@@ -2171,22 +2559,30 @@
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E54" t="s">
         <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>102</v>
-      </c>
-      <c r="H54" t="str">
-        <f t="shared" si="0"/>
-        <v>(53,3,'US Gov Arizona','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G54">
+        <f t="shared" ca="1" si="1"/>
+        <v>-44</v>
+      </c>
+      <c r="H54">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J54" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(53,3,'US Gov Arizona','Amérique du Nord','etats-Unis','-44','14'),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B55">
         <v>54</v>
@@ -2195,22 +2591,30 @@
         <v>3</v>
       </c>
       <c r="D55" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="E55" t="s">
         <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>102</v>
-      </c>
-      <c r="H55" t="str">
-        <f t="shared" si="0"/>
-        <v>(54,3,'South Central US','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G55">
+        <f t="shared" ca="1" si="1"/>
+        <v>89</v>
+      </c>
+      <c r="H55">
+        <f t="shared" ca="1" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="J55" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(54,3,'South Central US','Amérique du Nord','etats-Unis','89','24'),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B56">
         <v>55</v>
@@ -2219,22 +2623,29 @@
         <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="E56" t="s">
         <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>102</v>
-      </c>
-      <c r="H56" t="str">
-        <f t="shared" si="0"/>
-        <v>(55,3,'US Gov Texas','Amérique du Nord','etats-Unis'),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
+        <v>88</v>
+      </c>
+      <c r="G56" s="6">
+        <v>-97.8</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ca="1" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="J56" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(55,3,'US Gov Texas','Amérique du Nord','etats-Unis','-97.8','34'),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B57">
         <v>56</v>
@@ -2243,22 +2654,30 @@
         <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E57" t="s">
         <v>29</v>
       </c>
       <c r="F57" t="s">
-        <v>82</v>
-      </c>
-      <c r="H57" t="str">
-        <f t="shared" si="0"/>
-        <v>(56,3,'Brazil South','Amérique du Sud','Brésil'),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
+        <v>68</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ca="1" si="1"/>
+        <v>-76</v>
+      </c>
+      <c r="H57">
+        <f t="shared" ca="1" si="2"/>
+        <v>-26</v>
+      </c>
+      <c r="J57" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(56,3,'Brazil South','Amérique du Sud','Brésil','-76','-26'),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B58">
         <v>57</v>
@@ -2267,22 +2686,30 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="E58" t="s">
         <v>25</v>
       </c>
       <c r="F58" t="s">
-        <v>117</v>
-      </c>
-      <c r="H58" t="str">
-        <f t="shared" si="0"/>
-        <v>(57,3,'Norway West','Europe','Norvège'),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
+        <v>103</v>
+      </c>
+      <c r="G58">
+        <f t="shared" ca="1" si="1"/>
+        <v>-81</v>
+      </c>
+      <c r="H58">
+        <f t="shared" ca="1" si="2"/>
+        <v>-41</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(57,3,'Norway West','Europe','Norvège','-81','-41'),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B59">
         <v>58</v>
@@ -2291,22 +2718,30 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="E59" t="s">
         <v>25</v>
       </c>
       <c r="F59" t="s">
-        <v>65</v>
-      </c>
-      <c r="H59" t="str">
-        <f t="shared" si="0"/>
-        <v>(58,3,'West Europe','Europe','Pays-Bas'),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
+        <v>56</v>
+      </c>
+      <c r="G59">
+        <f t="shared" ca="1" si="1"/>
+        <v>-70</v>
+      </c>
+      <c r="H59">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(58,3,'West Europe','Europe','Pays-Bas','-70','6'),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B60">
         <v>59</v>
@@ -2315,7 +2750,7 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="E60" t="s">
         <v>25</v>
@@ -2323,14 +2758,22 @@
       <c r="F60" t="s">
         <v>39</v>
       </c>
-      <c r="H60" t="str">
-        <f t="shared" si="0"/>
-        <v>(59,3,'UK South','Europe','Grande-Bretagne'),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8">
+      <c r="G60">
+        <f t="shared" ca="1" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="H60">
+        <f t="shared" ca="1" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(59,3,'UK South','Europe','Grande-Bretagne','117','19'),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B61">
         <v>60</v>
@@ -2339,7 +2782,7 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="E61" t="s">
         <v>25</v>
@@ -2347,14 +2790,22 @@
       <c r="F61" t="s">
         <v>38</v>
       </c>
-      <c r="H61" t="str">
-        <f t="shared" si="0"/>
-        <v>(60,3,'North Europe','Europe','Irlande'),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8">
+      <c r="G61">
+        <f t="shared" ca="1" si="1"/>
+        <v>-98</v>
+      </c>
+      <c r="H61">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(60,3,'North Europe','Europe','Irlande','-98','9'),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B62">
         <v>61</v>
@@ -2363,7 +2814,7 @@
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="E62" t="s">
         <v>25</v>
@@ -2371,14 +2822,22 @@
       <c r="F62" t="s">
         <v>39</v>
       </c>
-      <c r="H62" t="str">
-        <f t="shared" si="0"/>
-        <v>(61,3,'UK West','Europe','Grande-Bretagne'),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8">
+      <c r="G62">
+        <f t="shared" ca="1" si="1"/>
+        <v>-163</v>
+      </c>
+      <c r="H62">
+        <f t="shared" ca="1" si="2"/>
+        <v>-26</v>
+      </c>
+      <c r="J62" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(61,3,'UK West','Europe','Grande-Bretagne','-163','-26'),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B63">
         <v>62</v>
@@ -2387,7 +2846,7 @@
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="E63" t="s">
         <v>25</v>
@@ -2395,14 +2854,22 @@
       <c r="F63" t="s">
         <v>40</v>
       </c>
-      <c r="H63" t="str">
-        <f t="shared" si="0"/>
-        <v>(62,3,'France Central','Europe','France'),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8">
+      <c r="G63">
+        <f t="shared" ca="1" si="1"/>
+        <v>-46</v>
+      </c>
+      <c r="H63">
+        <f t="shared" ca="1" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="J63" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(62,3,'France Central','Europe','France','-46','-11'),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B64">
         <v>63</v>
@@ -2411,7 +2878,7 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="E64" t="s">
         <v>25</v>
@@ -2419,14 +2886,22 @@
       <c r="F64" t="s">
         <v>40</v>
       </c>
-      <c r="H64" t="str">
-        <f t="shared" si="0"/>
-        <v>(63,3,'France South','Europe','France'),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="G64">
+        <f t="shared" ca="1" si="1"/>
+        <v>-18</v>
+      </c>
+      <c r="H64">
+        <f t="shared" ca="1" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="J64" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(63,3,'France South','Europe','France','-18','-11'),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B65">
         <v>64</v>
@@ -2435,22 +2910,30 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E65" t="s">
         <v>25</v>
       </c>
       <c r="F65" t="s">
-        <v>83</v>
-      </c>
-      <c r="H65" t="str">
-        <f t="shared" si="0"/>
-        <v>(64,3,'Switzerland West','Europe','Suisse'),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8">
+        <v>69</v>
+      </c>
+      <c r="G65">
+        <f t="shared" ca="1" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="H65">
+        <f t="shared" ca="1" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="J65" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(64,3,'Switzerland West','Europe','Suisse','111','-3'),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B66">
         <v>65</v>
@@ -2459,22 +2942,30 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="E66" t="s">
         <v>25</v>
       </c>
       <c r="F66" t="s">
-        <v>83</v>
-      </c>
-      <c r="H66" t="str">
-        <f t="shared" si="0"/>
-        <v>(65,3,'Switzerland North','Europe','Suisse'),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8">
+        <v>69</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ca="1" si="1"/>
+        <v>-105</v>
+      </c>
+      <c r="H66">
+        <f t="shared" ca="1" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="J66" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>(65,3,'Switzerland North','Europe','Suisse','-105','-50'),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B67">
         <v>66</v>
@@ -2483,7 +2974,7 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -2491,14 +2982,22 @@
       <c r="F67" t="s">
         <v>37</v>
       </c>
-      <c r="H67" t="str">
-        <f t="shared" ref="H67:H92" si="1">CONCATENATE("(",B67,",",C67,",'",D67,"','",E67,"','",F67,"'),")</f>
-        <v>(66,3,'Germany Central','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="G67">
+        <f t="shared" ca="1" si="1"/>
+        <v>-151</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ca="1" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="J67" t="str">
+        <f t="shared" ref="J67:J92" ca="1" si="3">CONCATENATE("(",B67,",",C67,",'",D67,"','",E67,"','",F67,"','",G67,"','",H67,"'),")</f>
+        <v>(66,3,'Germany Central','Europe','Allemagne','-151','-7'),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>67</v>
@@ -2507,7 +3006,7 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="E68" t="s">
         <v>25</v>
@@ -2515,14 +3014,22 @@
       <c r="F68" t="s">
         <v>37</v>
       </c>
-      <c r="H68" t="str">
-        <f t="shared" si="1"/>
-        <v>(67,3,'Germany Northeast','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8">
+      <c r="G68">
+        <f t="shared" ca="1" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="H68">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="J68" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(67,3,'Germany Northeast','Europe','Allemagne','180','14'),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B69">
         <v>68</v>
@@ -2531,7 +3038,7 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E69" t="s">
         <v>25</v>
@@ -2539,14 +3046,22 @@
       <c r="F69" t="s">
         <v>37</v>
       </c>
-      <c r="H69" t="str">
-        <f t="shared" si="1"/>
-        <v>(68,3,'Germany North','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
+      <c r="G69">
+        <f t="shared" ca="1" si="1"/>
+        <v>-94</v>
+      </c>
+      <c r="H69">
+        <f t="shared" ca="1" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="J69" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(68,3,'Germany North','Europe','Allemagne','-94','-16'),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B70">
         <v>69</v>
@@ -2555,7 +3070,7 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E70" t="s">
         <v>25</v>
@@ -2563,14 +3078,22 @@
       <c r="F70" t="s">
         <v>37</v>
       </c>
-      <c r="H70" t="str">
-        <f t="shared" si="1"/>
-        <v>(69,3,'Germany West Central','Europe','Allemagne'),</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
+      <c r="G70">
+        <f t="shared" ca="1" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="H70">
+        <f t="shared" ca="1" si="2"/>
+        <v>-46</v>
+      </c>
+      <c r="J70" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(69,3,'Germany West Central','Europe','Allemagne','129','-46'),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B71">
         <v>70</v>
@@ -2579,22 +3102,30 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E71" t="s">
         <v>25</v>
       </c>
       <c r="F71" t="s">
-        <v>117</v>
-      </c>
-      <c r="H71" t="str">
-        <f t="shared" si="1"/>
-        <v>(70,3,'Norway East','Europe','Norvège'),</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8">
+        <v>103</v>
+      </c>
+      <c r="G71">
+        <f t="shared" ref="G71:G92" ca="1" si="4">RANDBETWEEN(-180,180)</f>
+        <v>-97</v>
+      </c>
+      <c r="H71">
+        <f t="shared" ref="H71:H92" ca="1" si="5">RANDBETWEEN(-50,50)</f>
+        <v>-42</v>
+      </c>
+      <c r="J71" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(70,3,'Norway East','Europe','Norvège','-97','-42'),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B72">
         <v>71</v>
@@ -2603,22 +3134,30 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E72" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F72" t="s">
-        <v>121</v>
-      </c>
-      <c r="H72" t="str">
-        <f t="shared" si="1"/>
-        <v>(71,3,'South Africa West','Afrique','Afrique du Sud'),</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="G72">
+        <f t="shared" ca="1" si="4"/>
+        <v>69</v>
+      </c>
+      <c r="H72">
+        <f t="shared" ca="1" si="5"/>
+        <v>-38</v>
+      </c>
+      <c r="J72" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(71,3,'South Africa West','Afrique','Afrique du Sud','69','-38'),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B73">
         <v>72</v>
@@ -2627,22 +3166,30 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E73" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F73" t="s">
-        <v>121</v>
-      </c>
-      <c r="H73" t="str">
-        <f t="shared" si="1"/>
-        <v>(72,3,'South Africa North','Afrique','Afrique du Sud'),</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8">
+        <v>107</v>
+      </c>
+      <c r="G73">
+        <f t="shared" ca="1" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="H73">
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="J73" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(72,3,'South Africa North','Afrique','Afrique du Sud','23','15'),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B74">
         <v>73</v>
@@ -2651,22 +3198,30 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E74" t="s">
         <v>28</v>
       </c>
       <c r="F74" t="s">
-        <v>141</v>
-      </c>
-      <c r="H74" t="str">
-        <f t="shared" si="1"/>
-        <v>(73,3,'UAE Central','Asie-Pacifique','Emirats Arabes Unis'),</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
+        <v>127</v>
+      </c>
+      <c r="G74">
+        <f t="shared" ca="1" si="4"/>
+        <v>-146</v>
+      </c>
+      <c r="H74">
+        <f t="shared" ca="1" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="J74" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(73,3,'UAE Central','Asie-Pacifique','Emirats Arabes Unis','-146','28'),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B75">
         <v>74</v>
@@ -2675,22 +3230,30 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="E75" t="s">
         <v>28</v>
       </c>
       <c r="F75" t="s">
-        <v>141</v>
-      </c>
-      <c r="H75" t="str">
-        <f t="shared" si="1"/>
-        <v>(74,3,'UAE North','Asie-Pacifique','Emirats Arabes Unis'),</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8">
+        <v>127</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ca="1" si="4"/>
+        <v>178</v>
+      </c>
+      <c r="H75">
+        <f t="shared" ca="1" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="J75" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(74,3,'UAE North','Asie-Pacifique','Emirats Arabes Unis','178','30'),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B76">
         <v>75</v>
@@ -2699,7 +3262,7 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="E76" t="s">
         <v>28</v>
@@ -2707,14 +3270,22 @@
       <c r="F76" t="s">
         <v>33</v>
       </c>
-      <c r="H76" t="str">
-        <f t="shared" si="1"/>
-        <v>(75,3,'West India','Asie-Pacifique','Inde'),</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="G76">
+        <f t="shared" ca="1" si="4"/>
+        <v>-171</v>
+      </c>
+      <c r="H76">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="J76" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(75,3,'West India','Asie-Pacifique','Inde','-171','19'),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B77">
         <v>76</v>
@@ -2723,7 +3294,7 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E77" t="s">
         <v>28</v>
@@ -2731,14 +3302,22 @@
       <c r="F77" t="s">
         <v>33</v>
       </c>
-      <c r="H77" t="str">
-        <f t="shared" si="1"/>
-        <v>(76,3,'Central India','Asie-Pacifique','Inde'),</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="G77">
+        <f t="shared" ca="1" si="4"/>
+        <v>-64</v>
+      </c>
+      <c r="H77">
+        <f t="shared" ca="1" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="J77" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(76,3,'Central India','Asie-Pacifique','Inde','-64','-10'),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B78">
         <v>77</v>
@@ -2747,7 +3326,7 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="E78" t="s">
         <v>28</v>
@@ -2755,14 +3334,22 @@
       <c r="F78" t="s">
         <v>33</v>
       </c>
-      <c r="H78" t="str">
-        <f t="shared" si="1"/>
-        <v>(77,3,'South India','Asie-Pacifique','Inde'),</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="G78">
+        <f t="shared" ca="1" si="4"/>
+        <v>116</v>
+      </c>
+      <c r="H78">
+        <f t="shared" ca="1" si="5"/>
+        <v>-16</v>
+      </c>
+      <c r="J78" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(77,3,'South India','Asie-Pacifique','Inde','116','-16'),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B79">
         <v>78</v>
@@ -2771,22 +3358,30 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E79" t="s">
         <v>28</v>
       </c>
       <c r="F79" t="s">
-        <v>78</v>
-      </c>
-      <c r="H79" t="str">
-        <f t="shared" si="1"/>
-        <v>(78,3,'Southeast Asia','Asie-Pacifique','Singapour'),</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
+        <v>65</v>
+      </c>
+      <c r="G79">
+        <f t="shared" ca="1" si="4"/>
+        <v>105</v>
+      </c>
+      <c r="H79">
+        <f t="shared" ca="1" si="5"/>
+        <v>-25</v>
+      </c>
+      <c r="J79" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(78,3,'Southeast Asia','Asie-Pacifique','Singapour','105','-25'),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B80">
         <v>79</v>
@@ -2795,22 +3390,30 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E80" t="s">
         <v>28</v>
       </c>
       <c r="F80" t="s">
-        <v>142</v>
-      </c>
-      <c r="H80" t="str">
-        <f t="shared" si="1"/>
-        <v>(79,3,'China North','Asie-Pacifique','Chine'),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
+        <v>128</v>
+      </c>
+      <c r="G80">
+        <f t="shared" ca="1" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="H80">
+        <f t="shared" ca="1" si="5"/>
+        <v>-3</v>
+      </c>
+      <c r="J80" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(79,3,'China North','Asie-Pacifique','Chine','7','-3'),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B81">
         <v>80</v>
@@ -2819,22 +3422,30 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="E81" t="s">
         <v>28</v>
       </c>
       <c r="F81" t="s">
-        <v>142</v>
-      </c>
-      <c r="H81" t="str">
-        <f t="shared" si="1"/>
-        <v>(80,3,'China North 2','Asie-Pacifique','Chine'),</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
+        <v>128</v>
+      </c>
+      <c r="G81">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="H81">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J81" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(80,3,'China North 2','Asie-Pacifique','Chine','5','0'),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B82">
         <v>81</v>
@@ -2843,7 +3454,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E82" t="s">
         <v>28</v>
@@ -2851,14 +3462,22 @@
       <c r="F82" t="s">
         <v>35</v>
       </c>
-      <c r="H82" t="str">
-        <f t="shared" si="1"/>
-        <v>(81,3,'Korea Central','Asie-Pacifique','Corée du Sud'),</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="G82">
+        <f t="shared" ca="1" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="H82">
+        <f t="shared" ca="1" si="5"/>
+        <v>-36</v>
+      </c>
+      <c r="J82" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(81,3,'Korea Central','Asie-Pacifique','Corée du Sud','99','-36'),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B83">
         <v>82</v>
@@ -2867,7 +3486,7 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E83" t="s">
         <v>28</v>
@@ -2875,14 +3494,22 @@
       <c r="F83" t="s">
         <v>35</v>
       </c>
-      <c r="H83" t="str">
-        <f t="shared" si="1"/>
-        <v>(82,3,'Korea South','Asie-Pacifique','Corée du Sud'),</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="G83">
+        <f t="shared" ca="1" si="4"/>
+        <v>-79</v>
+      </c>
+      <c r="H83">
+        <f t="shared" ca="1" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="J83" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(82,3,'Korea South','Asie-Pacifique','Corée du Sud','-79','35'),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B84">
         <v>83</v>
@@ -2891,22 +3518,30 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E84" t="s">
         <v>28</v>
       </c>
       <c r="F84" t="s">
-        <v>142</v>
-      </c>
-      <c r="H84" t="str">
-        <f t="shared" si="1"/>
-        <v>(83,3,'China East','Asie-Pacifique','Chine'),</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
+        <v>128</v>
+      </c>
+      <c r="G84">
+        <f t="shared" ca="1" si="4"/>
+        <v>-40</v>
+      </c>
+      <c r="H84">
+        <f t="shared" ca="1" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="J84" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(83,3,'China East','Asie-Pacifique','Chine','-40','-10'),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B85">
         <v>84</v>
@@ -2915,22 +3550,30 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E85" t="s">
         <v>28</v>
       </c>
       <c r="F85" t="s">
-        <v>142</v>
-      </c>
-      <c r="H85" t="str">
-        <f t="shared" si="1"/>
-        <v>(84,3,'China East 2','Asie-Pacifique','Chine'),</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
+        <v>128</v>
+      </c>
+      <c r="G85">
+        <f t="shared" ca="1" si="4"/>
+        <v>-104</v>
+      </c>
+      <c r="H85">
+        <f t="shared" ca="1" si="5"/>
+        <v>-25</v>
+      </c>
+      <c r="J85" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(84,3,'China East 2','Asie-Pacifique','Chine','-104','-25'),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B86">
         <v>85</v>
@@ -2939,22 +3582,30 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E86" t="s">
         <v>28</v>
       </c>
       <c r="F86" t="s">
-        <v>142</v>
-      </c>
-      <c r="H86" t="str">
-        <f t="shared" si="1"/>
-        <v>(85,3,'East Asia','Asie-Pacifique','Chine'),</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
+        <v>128</v>
+      </c>
+      <c r="G86">
+        <f t="shared" ca="1" si="4"/>
+        <v>-97</v>
+      </c>
+      <c r="H86">
+        <f t="shared" ca="1" si="5"/>
+        <v>-10</v>
+      </c>
+      <c r="J86" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(85,3,'East Asia','Asie-Pacifique','Chine','-97','-10'),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B87">
         <v>86</v>
@@ -2963,7 +3614,7 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E87" t="s">
         <v>28</v>
@@ -2971,14 +3622,22 @@
       <c r="F87" t="s">
         <v>34</v>
       </c>
-      <c r="H87" t="str">
-        <f t="shared" si="1"/>
-        <v>(86,3,'Japan East','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="G87">
+        <f t="shared" ca="1" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="H87">
+        <f t="shared" ca="1" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="J87" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(86,3,'Japan East','Asie-Pacifique','Japon','18','44'),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B88">
         <v>87</v>
@@ -2987,7 +3646,7 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E88" t="s">
         <v>28</v>
@@ -2995,14 +3654,22 @@
       <c r="F88" t="s">
         <v>34</v>
       </c>
-      <c r="H88" t="str">
-        <f t="shared" si="1"/>
-        <v>(87,3,'Japan West','Asie-Pacifique','Japon'),</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="G88">
+        <f t="shared" ca="1" si="4"/>
+        <v>-45</v>
+      </c>
+      <c r="H88">
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="J88" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(87,3,'Japan West','Asie-Pacifique','Japon','-45','19'),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B89">
         <v>88</v>
@@ -3011,7 +3678,7 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E89" t="s">
         <v>28</v>
@@ -3019,14 +3686,22 @@
       <c r="F89" t="s">
         <v>36</v>
       </c>
-      <c r="H89" t="str">
-        <f t="shared" si="1"/>
-        <v>(88,3,'Australia East','Asie-Pacifique','Australie'),</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="G89">
+        <f t="shared" ca="1" si="4"/>
+        <v>-40</v>
+      </c>
+      <c r="H89">
+        <f t="shared" ca="1" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="J89" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(88,3,'Australia East','Asie-Pacifique','Australie','-40','45'),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B90">
         <v>89</v>
@@ -3035,7 +3710,7 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E90" t="s">
         <v>28</v>
@@ -3043,14 +3718,22 @@
       <c r="F90" t="s">
         <v>36</v>
       </c>
-      <c r="H90" t="str">
-        <f t="shared" si="1"/>
-        <v>(89,3,'Australia Southeast','Asie-Pacifique','Australie'),</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="G90">
+        <f t="shared" ca="1" si="4"/>
+        <v>-137</v>
+      </c>
+      <c r="H90">
+        <f t="shared" ca="1" si="5"/>
+        <v>-45</v>
+      </c>
+      <c r="J90" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(89,3,'Australia Southeast','Asie-Pacifique','Australie','-137','-45'),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B91">
         <v>90</v>
@@ -3059,7 +3742,7 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E91" t="s">
         <v>28</v>
@@ -3067,14 +3750,22 @@
       <c r="F91" t="s">
         <v>36</v>
       </c>
-      <c r="H91" t="str">
-        <f t="shared" si="1"/>
-        <v>(90,3,'Australia Central','Asie-Pacifique','Australie'),</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="G91">
+        <f t="shared" ca="1" si="4"/>
+        <v>119</v>
+      </c>
+      <c r="H91">
+        <f t="shared" ca="1" si="5"/>
+        <v>-47</v>
+      </c>
+      <c r="J91" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(90,3,'Australia Central','Asie-Pacifique','Australie','119','-47'),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B92">
         <v>91</v>
@@ -3083,7 +3774,7 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E92" t="s">
         <v>28</v>
@@ -3091,12 +3782,21 @@
       <c r="F92" t="s">
         <v>36</v>
       </c>
-      <c r="H92" t="str">
-        <f t="shared" si="1"/>
-        <v>(91,3,'Australia Central 2','Asie-Pacifique','Australie'),</v>
+      <c r="G92">
+        <f t="shared" ca="1" si="4"/>
+        <v>125</v>
+      </c>
+      <c r="H92">
+        <f t="shared" ca="1" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="J92" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>(91,3,'Australia Central 2','Asie-Pacifique','Australie','125','32'),</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J92" xr:uid="{B13B48CD-DB70-48DF-9873-24BF54116718}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3107,7 +3807,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C19" sqref="C18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -3115,192 +3815,110 @@
     <col min="2" max="2" width="21.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" thickBot="1">
-      <c r="A1" s="1" t="s">
-        <v>27</v>
-      </c>
+    <row r="1" spans="1:3" ht="15" thickBot="1">
+      <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="19.8" thickBot="1">
+    <row r="2" spans="1:3" ht="15" thickBot="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>43</v>
-      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="15" thickBot="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="15" thickBot="1">
       <c r="A4" s="2"/>
-      <c r="B4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" ht="15" thickBot="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" ht="15" thickBot="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="15" thickBot="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>57</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>59</v>
-      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" ht="15" thickBot="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>61</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" ht="15" thickBot="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" ht="15" thickBot="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" ht="15" thickBot="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="19.8" thickBot="1">
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="15" thickBot="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="19.8" thickBot="1">
+      <c r="B17" s="3"/>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" thickBot="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" ht="15" thickBot="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" ht="15" thickBot="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1">
       <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>80</v>
-      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
correct coordinates for storage locations
</commit_message>
<xml_diff>
--- a/data/db/data providers.xlsx
+++ b/data/db/data providers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082617F9-86FA-4CB1-B59F-23B7EAF37C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA10EA1-9449-487E-858B-756D14833560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="131">
   <si>
     <t>Amazon</t>
   </si>
@@ -301,9 +301,6 @@
   </si>
   <si>
     <t>Brazil South</t>
-  </si>
-  <si>
-    <t>etats-Unis</t>
   </si>
   <si>
     <t>Norway West</t>
@@ -852,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC19A3D-01C7-400F-ABF6-368E3B90A145}">
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="H80" sqref="H80"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K71" sqref="K71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -868,7 +865,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s">
         <v>20</v>
@@ -886,10 +883,10 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H1" t="s">
         <v>130</v>
-      </c>
-      <c r="H1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -1031,17 +1028,15 @@
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="G6">
-        <f ca="1">RANDBETWEEN(-180,180)</f>
-        <v>62</v>
-      </c>
-      <c r="H6">
-        <f ca="1">RANDBETWEEN(-50,50)</f>
-        <v>14</v>
+      <c r="G6" s="6">
+        <v>114</v>
+      </c>
+      <c r="H6" s="6">
+        <v>22</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(5,1,'Asia Pacific (Hong Kong)','Asie-Pacifique','Hong Kong','62','14'),</v>
+        <f t="shared" si="0"/>
+        <v>(5,1,'Asia Pacific (Hong Kong)','Asie-Pacifique','Hong Kong','114','22'),</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1063,17 +1058,15 @@
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7">
-        <f t="shared" ref="G7:G70" ca="1" si="1">RANDBETWEEN(-180,180)</f>
-        <v>41</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H70" ca="1" si="2">RANDBETWEEN(-50,50)</f>
-        <v>4</v>
+      <c r="G7" s="6">
+        <v>73</v>
+      </c>
+      <c r="H7" s="6">
+        <v>19</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(6,1,'Asia Pacific (Mumbai)','Asie-Pacifique','Inde','41','4'),</v>
+        <f t="shared" si="0"/>
+        <v>(6,1,'Asia Pacific (Mumbai)','Asie-Pacifique','Inde','73','19'),</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1095,17 +1088,15 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8">
-        <f t="shared" ca="1" si="1"/>
-        <v>-70</v>
-      </c>
-      <c r="H8">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+      <c r="G8" s="6">
+        <v>136</v>
+      </c>
+      <c r="H8" s="6">
+        <v>35</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(7,1,'Asia Pacific (Osaka-Local)','Asie-Pacifique','Japon','-70','34'),</v>
+        <f t="shared" si="0"/>
+        <v>(7,1,'Asia Pacific (Osaka-Local)','Asie-Pacifique','Japon','136','35'),</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1127,17 +1118,15 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9">
-        <f t="shared" ca="1" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="H9">
-        <f t="shared" ca="1" si="2"/>
-        <v>47</v>
+      <c r="G9" s="6">
+        <v>127</v>
+      </c>
+      <c r="H9" s="6">
+        <v>37</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(8,1,'Asia Pacific (Seoul)','Asie-Pacifique','Corée du Sud','162','47'),</v>
+        <f t="shared" si="0"/>
+        <v>(8,1,'Asia Pacific (Seoul)','Asie-Pacifique','Corée du Sud','127','37'),</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1159,17 +1148,15 @@
       <c r="F10" t="s">
         <v>65</v>
       </c>
-      <c r="G10">
-        <f t="shared" ca="1" si="1"/>
-        <v>-49</v>
-      </c>
-      <c r="H10">
-        <f t="shared" ca="1" si="2"/>
-        <v>-13</v>
+      <c r="G10" s="6">
+        <v>103.7</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1.4</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(9,1,'Asia Pacific (Singapore)','Asie-Pacifique','Singapour','-49','-13'),</v>
+        <f t="shared" si="0"/>
+        <v>(9,1,'Asia Pacific (Singapore)','Asie-Pacifique','Singapour','103.7','1.4'),</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1191,17 +1178,15 @@
       <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="G11">
-        <f t="shared" ca="1" si="1"/>
-        <v>-71</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ca="1" si="2"/>
-        <v>25</v>
+      <c r="G11" s="6">
+        <v>151</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-34</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(10,1,'Asia Pacific (Sydney)','Asie-Pacifique','Australie','-71','25'),</v>
+        <f t="shared" si="0"/>
+        <v>(10,1,'Asia Pacific (Sydney)','Asie-Pacifique','Australie','151','-34'),</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1223,17 +1208,15 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="G12">
-        <f t="shared" ca="1" si="1"/>
-        <v>-158</v>
-      </c>
-      <c r="H12">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+      <c r="G12" s="6">
+        <v>140</v>
+      </c>
+      <c r="H12" s="6">
+        <v>36</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(11,1,'Asia Pacific (Tokyo)','Asie-Pacifique','Japon','-158','3'),</v>
+        <f t="shared" si="0"/>
+        <v>(11,1,'Asia Pacific (Tokyo)','Asie-Pacifique','Japon','140','36'),</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1255,17 +1238,15 @@
       <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="G13">
-        <f t="shared" ca="1" si="1"/>
-        <v>163</v>
-      </c>
-      <c r="H13">
-        <f t="shared" ca="1" si="2"/>
-        <v>-24</v>
+      <c r="G13" s="6">
+        <v>-99</v>
+      </c>
+      <c r="H13" s="6">
+        <v>52</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(12,1,'Canada (Central)','Amérique du Nord','Canada','163','-24'),</v>
+        <f t="shared" si="0"/>
+        <v>(12,1,'Canada (Central)','Amérique du Nord','Canada','-99','52'),</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1287,17 +1268,15 @@
       <c r="F14" t="s">
         <v>37</v>
       </c>
-      <c r="G14">
-        <f t="shared" ca="1" si="1"/>
-        <v>128</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+      <c r="G14" s="6">
+        <v>9</v>
+      </c>
+      <c r="H14" s="6">
+        <v>50</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(13,1,'Europe (Frankfurt)','Europe','Allemagne','128','14'),</v>
+        <f t="shared" si="0"/>
+        <v>(13,1,'Europe (Frankfurt)','Europe','Allemagne','9','50'),</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1319,17 +1298,15 @@
       <c r="F15" t="s">
         <v>38</v>
       </c>
-      <c r="G15">
-        <f t="shared" ca="1" si="1"/>
-        <v>-46</v>
-      </c>
-      <c r="H15">
-        <f t="shared" ca="1" si="2"/>
-        <v>27</v>
+      <c r="G15" s="6">
+        <v>-7</v>
+      </c>
+      <c r="H15" s="6">
+        <v>53</v>
       </c>
       <c r="J15" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(14,1,'Europe (Ireland)','Europe','Irlande','-46','27'),</v>
+        <f t="shared" si="0"/>
+        <v>(14,1,'Europe (Ireland)','Europe','Irlande','-7','53'),</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1351,17 +1328,15 @@
       <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="G16">
-        <f t="shared" ca="1" si="1"/>
-        <v>66</v>
-      </c>
-      <c r="H16">
-        <f t="shared" ca="1" si="2"/>
-        <v>45</v>
+      <c r="G16" s="6">
+        <v>-0.4</v>
+      </c>
+      <c r="H16" s="6">
+        <v>51</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(15,1,'Europe (London)','Europe','Grande-Bretagne','66','45'),</v>
+        <f t="shared" si="0"/>
+        <v>(15,1,'Europe (London)','Europe','Grande-Bretagne','-0.4','51'),</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1383,17 +1358,15 @@
       <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="G17">
-        <f t="shared" ca="1" si="1"/>
-        <v>-179</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+      <c r="G17" s="6">
+        <v>3</v>
+      </c>
+      <c r="H17" s="6">
+        <v>49</v>
       </c>
       <c r="J17" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(16,1,'Europe (Paris)','Europe','France','-179','4'),</v>
+        <f t="shared" si="0"/>
+        <v>(16,1,'Europe (Paris)','Europe','France','3','49'),</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1415,17 +1388,15 @@
       <c r="F18" t="s">
         <v>41</v>
       </c>
-      <c r="G18">
-        <f t="shared" ca="1" si="1"/>
-        <v>179</v>
-      </c>
-      <c r="H18">
-        <f t="shared" ca="1" si="2"/>
-        <v>33</v>
+      <c r="G18" s="6">
+        <v>18</v>
+      </c>
+      <c r="H18" s="6">
+        <v>60</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(17,1,'Europe (Stockholm)','Europe','Suède','179','33'),</v>
+        <f t="shared" si="0"/>
+        <v>(17,1,'Europe (Stockholm)','Europe','Suède','18','60'),</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1447,17 +1418,15 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>-36</v>
-      </c>
-      <c r="H19">
-        <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+      <c r="G19" s="6">
+        <v>50.5</v>
+      </c>
+      <c r="H19" s="6">
+        <v>25.9</v>
       </c>
       <c r="J19" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(18,1,'Middle East (Bahrain)','Asie-Pacifique','Bahrain','-36','28'),</v>
+        <f t="shared" si="0"/>
+        <v>(18,1,'Middle East (Bahrain)','Asie-Pacifique','Bahrain','50.5','25.9'),</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1479,17 +1448,15 @@
       <c r="F20" t="s">
         <v>68</v>
       </c>
-      <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>-25</v>
-      </c>
-      <c r="H20">
-        <f t="shared" ca="1" si="2"/>
-        <v>46</v>
+      <c r="G20" s="6">
+        <v>-46</v>
+      </c>
+      <c r="H20" s="6">
+        <v>-23</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(19,1,'South America (São Paulo)','Amérique du Sud','Brésil','-25','46'),</v>
+        <f t="shared" si="0"/>
+        <v>(19,1,'South America (São Paulo)','Amérique du Sud','Brésil','-46','-23'),</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1511,17 +1478,15 @@
       <c r="F21" t="s">
         <v>24</v>
       </c>
-      <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>62</v>
-      </c>
-      <c r="H21">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+      <c r="G21" s="6">
+        <v>-66</v>
+      </c>
+      <c r="H21" s="6">
+        <v>46</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(20,2,'NORTHAMERICA-NORTHEAST1','Amérique du Nord','Canada','62','3'),</v>
+        <f t="shared" si="0"/>
+        <v>(20,2,'NORTHAMERICA-NORTHEAST1','Amérique du Nord','Canada','-66','46'),</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1543,17 +1508,15 @@
       <c r="F22" t="s">
         <v>30</v>
       </c>
-      <c r="G22">
-        <f t="shared" ca="1" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="H22">
-        <f t="shared" ca="1" si="2"/>
-        <v>29</v>
+      <c r="G22" s="6">
+        <v>-97</v>
+      </c>
+      <c r="H22" s="6">
+        <v>42</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(21,2,'US-CENTRAL1','Amérique du Nord','Etats-Unis','46','29'),</v>
+        <f t="shared" si="0"/>
+        <v>(21,2,'US-CENTRAL1','Amérique du Nord','Etats-Unis','-97','42'),</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1575,17 +1538,15 @@
       <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="G23">
-        <f t="shared" ca="1" si="1"/>
-        <v>-92</v>
-      </c>
-      <c r="H23">
-        <f t="shared" ca="1" si="2"/>
-        <v>-43</v>
+      <c r="G23" s="6">
+        <v>-74</v>
+      </c>
+      <c r="H23" s="6">
+        <v>42</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(22,2,'US-EAST1','Amérique du Nord','Etats-Unis','-92','-43'),</v>
+        <f t="shared" si="0"/>
+        <v>(22,2,'US-EAST1','Amérique du Nord','Etats-Unis','-74','42'),</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1607,17 +1568,15 @@
       <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="G24">
-        <f t="shared" ca="1" si="1"/>
-        <v>-160</v>
-      </c>
-      <c r="H24">
-        <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+      <c r="G24" s="6">
+        <v>-77</v>
+      </c>
+      <c r="H24" s="6">
+        <v>40</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(23,2,'US-EAST4','Amérique du Nord','Etats-Unis','-160','11'),</v>
+        <f t="shared" si="0"/>
+        <v>(23,2,'US-EAST4','Amérique du Nord','Etats-Unis','-77','40'),</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1639,17 +1598,15 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
-      <c r="G25">
-        <f t="shared" ca="1" si="1"/>
-        <v>161</v>
-      </c>
-      <c r="H25">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+      <c r="G25" s="6">
+        <v>-122</v>
+      </c>
+      <c r="H25" s="6">
+        <v>41</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(24,2,'US-WEST1','Amérique du Nord','Etats-Unis','161','0'),</v>
+        <f t="shared" si="0"/>
+        <v>(24,2,'US-WEST1','Amérique du Nord','Etats-Unis','-122','41'),</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1671,17 +1628,15 @@
       <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="G26">
-        <f t="shared" ca="1" si="1"/>
-        <v>83</v>
-      </c>
-      <c r="H26">
-        <f t="shared" ca="1" si="2"/>
-        <v>-25</v>
+      <c r="G26" s="6">
+        <v>-116</v>
+      </c>
+      <c r="H26" s="6">
+        <v>34</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(25,2,'US-WEST2','Amérique du Nord','Etats-Unis','83','-25'),</v>
+        <f t="shared" si="0"/>
+        <v>(25,2,'US-WEST2','Amérique du Nord','Etats-Unis','-116','34'),</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1703,17 +1658,15 @@
       <c r="F27" t="s">
         <v>68</v>
       </c>
-      <c r="G27">
-        <f t="shared" ca="1" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="H27">
-        <f t="shared" ca="1" si="2"/>
-        <v>-34</v>
+      <c r="G27" s="6">
+        <v>-41</v>
+      </c>
+      <c r="H27" s="6">
+        <v>-14</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(26,2,'SOUTHAMERICA-EAST1','Amérique du Sud','Brésil','63','-34'),</v>
+        <f t="shared" si="0"/>
+        <v>(26,2,'SOUTHAMERICA-EAST1','Amérique du Sud','Brésil','-41','-14'),</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1735,17 +1688,15 @@
       <c r="F28" t="s">
         <v>50</v>
       </c>
-      <c r="G28">
-        <f t="shared" ca="1" si="1"/>
-        <v>95</v>
-      </c>
-      <c r="H28">
-        <f t="shared" ca="1" si="2"/>
-        <v>-22</v>
+      <c r="G28" s="6">
+        <v>25</v>
+      </c>
+      <c r="H28" s="6">
+        <v>61</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(27,2,'EUROPE-NORTH1','Europe','Finlande','95','-22'),</v>
+        <f t="shared" si="0"/>
+        <v>(27,2,'EUROPE-NORTH1','Europe','Finlande','25','61'),</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1767,17 +1718,15 @@
       <c r="F29" t="s">
         <v>52</v>
       </c>
-      <c r="G29">
-        <f t="shared" ca="1" si="1"/>
-        <v>143</v>
-      </c>
-      <c r="H29">
-        <f t="shared" ca="1" si="2"/>
-        <v>43</v>
+      <c r="G29" s="6">
+        <v>4</v>
+      </c>
+      <c r="H29" s="6">
+        <v>51</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(28,2,'EUROPE-WEST1','Europe','Belgique','143','43'),</v>
+        <f t="shared" si="0"/>
+        <v>(28,2,'EUROPE-WEST1','Europe','Belgique','4','51'),</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1799,17 +1748,15 @@
       <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="G30">
-        <f t="shared" ca="1" si="1"/>
-        <v>131</v>
-      </c>
-      <c r="H30">
-        <f t="shared" ca="1" si="2"/>
-        <v>-16</v>
+      <c r="G30" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="H30" s="6">
+        <v>52</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(29,2,'EUROPE-WEST2','Europe','Grande-Bretagne','131','-16'),</v>
+        <f t="shared" si="0"/>
+        <v>(29,2,'EUROPE-WEST2','Europe','Grande-Bretagne','-1.5','52'),</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1831,17 +1778,15 @@
       <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="G31">
-        <f t="shared" ca="1" si="1"/>
-        <v>133</v>
-      </c>
-      <c r="H31">
-        <f t="shared" ca="1" si="2"/>
-        <v>-32</v>
+      <c r="G31" s="6">
+        <v>7</v>
+      </c>
+      <c r="H31" s="6">
+        <v>50</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(30,2,'EUROPE-WEST3','Europe','Allemagne','133','-32'),</v>
+        <f t="shared" si="0"/>
+        <v>(30,2,'EUROPE-WEST3','Europe','Allemagne','7','50'),</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1863,17 +1808,15 @@
       <c r="F32" t="s">
         <v>56</v>
       </c>
-      <c r="G32">
-        <f t="shared" ca="1" si="1"/>
-        <v>116</v>
-      </c>
-      <c r="H32">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+      <c r="G32" s="6">
+        <v>5.3</v>
+      </c>
+      <c r="H32" s="6">
+        <v>52</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(31,2,'EUROPE-WEST4','Europe','Pays-Bas','116','34'),</v>
+        <f t="shared" si="0"/>
+        <v>(31,2,'EUROPE-WEST4','Europe','Pays-Bas','5.3','52'),</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1895,17 +1838,15 @@
       <c r="F33" t="s">
         <v>69</v>
       </c>
-      <c r="G33">
-        <f t="shared" ca="1" si="1"/>
-        <v>-122</v>
-      </c>
-      <c r="H33">
-        <f t="shared" ca="1" si="2"/>
-        <v>-48</v>
+      <c r="G33" s="6">
+        <v>8</v>
+      </c>
+      <c r="H33" s="6">
+        <v>47</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(32,2,'EUROPE-WEST6','Europe','Suisse','-122','-48'),</v>
+        <f t="shared" si="0"/>
+        <v>(32,2,'EUROPE-WEST6','Europe','Suisse','8','47'),</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1927,17 +1868,15 @@
       <c r="F34" t="s">
         <v>59</v>
       </c>
-      <c r="G34">
-        <f t="shared" ca="1" si="1"/>
-        <v>-119</v>
-      </c>
-      <c r="H34">
-        <f t="shared" ca="1" si="2"/>
-        <v>30</v>
+      <c r="G34" s="6">
+        <v>121</v>
+      </c>
+      <c r="H34" s="6">
+        <v>24</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(33,2,'ASIA-EAST1','Asie-Pacifique','Taïwan','-119','30'),</v>
+        <f t="shared" si="0"/>
+        <v>(33,2,'ASIA-EAST1','Asie-Pacifique','Taïwan','121','24'),</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1959,17 +1898,15 @@
       <c r="F35" t="s">
         <v>31</v>
       </c>
-      <c r="G35">
-        <f t="shared" ca="1" si="1"/>
-        <v>-53</v>
-      </c>
-      <c r="H35">
-        <f t="shared" ca="1" si="2"/>
-        <v>31</v>
+      <c r="G35" s="6">
+        <v>114</v>
+      </c>
+      <c r="H35" s="6">
+        <v>22</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(34,2,'ASIA-EAST2','Asie-Pacifique','Hong Kong','-53','31'),</v>
+        <f t="shared" si="0"/>
+        <v>(34,2,'ASIA-EAST2','Asie-Pacifique','Hong Kong','114','22'),</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1991,17 +1928,15 @@
       <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="G36">
-        <f t="shared" ca="1" si="1"/>
-        <v>177</v>
-      </c>
-      <c r="H36">
-        <f t="shared" ca="1" si="2"/>
-        <v>-17</v>
+      <c r="G36" s="6">
+        <v>139</v>
+      </c>
+      <c r="H36" s="6">
+        <v>36</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(35,2,'ASIA-NORTHEAST1','Asie-Pacifique','Japon','177','-17'),</v>
+        <f t="shared" si="0"/>
+        <v>(35,2,'ASIA-NORTHEAST1','Asie-Pacifique','Japon','139','36'),</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -2023,17 +1958,15 @@
       <c r="F37" t="s">
         <v>34</v>
       </c>
-      <c r="G37">
-        <f t="shared" ca="1" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="H37">
-        <f t="shared" ca="1" si="2"/>
-        <v>28</v>
+      <c r="G37" s="6">
+        <v>134</v>
+      </c>
+      <c r="H37" s="6">
+        <v>35</v>
       </c>
       <c r="J37" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(36,2,'ASIA-NORTHEAST2','Asie-Pacifique','Japon','162','28'),</v>
+        <f t="shared" si="0"/>
+        <v>(36,2,'ASIA-NORTHEAST2','Asie-Pacifique','Japon','134','35'),</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -2055,17 +1988,15 @@
       <c r="F38" t="s">
         <v>33</v>
       </c>
-      <c r="G38">
-        <f t="shared" ca="1" si="1"/>
-        <v>-39</v>
-      </c>
-      <c r="H38">
-        <f t="shared" ca="1" si="2"/>
-        <v>-10</v>
+      <c r="G38" s="6">
+        <v>78</v>
+      </c>
+      <c r="H38" s="6">
+        <v>11</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(37,2,'ASIA-SOUTH1','Asie-Pacifique','Inde','-39','-10'),</v>
+        <f t="shared" si="0"/>
+        <v>(37,2,'ASIA-SOUTH1','Asie-Pacifique','Inde','78','11'),</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -2087,17 +2018,15 @@
       <c r="F39" t="s">
         <v>65</v>
       </c>
-      <c r="G39">
-        <f t="shared" ca="1" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H39">
-        <f t="shared" ca="1" si="2"/>
-        <v>-9</v>
+      <c r="G39" s="6">
+        <v>103.7</v>
+      </c>
+      <c r="H39" s="6">
+        <v>1.4</v>
       </c>
       <c r="J39" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(38,2,'ASIA-SOUTHEAST1','Asie-Pacifique','Singapour','-100','-9'),</v>
+        <f t="shared" si="0"/>
+        <v>(38,2,'ASIA-SOUTHEAST1','Asie-Pacifique','Singapour','103.7','1.4'),</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -2119,17 +2048,15 @@
       <c r="F40" t="s">
         <v>36</v>
       </c>
-      <c r="G40">
-        <f t="shared" ca="1" si="1"/>
-        <v>169</v>
-      </c>
-      <c r="H40">
-        <f t="shared" ca="1" si="2"/>
-        <v>42</v>
+      <c r="G40" s="6">
+        <v>150</v>
+      </c>
+      <c r="H40" s="6">
+        <v>-36</v>
       </c>
       <c r="J40" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(39,2,'AUSTRALIA-SOUTHEAST1','Asie-Pacifique','Australie','169','42'),</v>
+        <f t="shared" si="0"/>
+        <v>(39,2,'AUSTRALIA-SOUTHEAST1','Asie-Pacifique','Australie','150','-36'),</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -2151,17 +2078,15 @@
       <c r="F41" t="s">
         <v>24</v>
       </c>
-      <c r="G41">
-        <f t="shared" ca="1" si="1"/>
-        <v>124</v>
-      </c>
-      <c r="H41">
-        <f t="shared" ca="1" si="2"/>
-        <v>36</v>
+      <c r="G41" s="6">
+        <v>-73</v>
+      </c>
+      <c r="H41" s="6">
+        <v>47</v>
       </c>
       <c r="J41" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(40,3,'Canada East','Amérique du Nord','Canada','124','36'),</v>
+        <f t="shared" si="0"/>
+        <v>(40,3,'Canada East','Amérique du Nord','Canada','-73','47'),</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -2183,17 +2108,15 @@
       <c r="F42" t="s">
         <v>24</v>
       </c>
-      <c r="G42">
-        <f t="shared" ca="1" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="H42">
-        <f t="shared" ca="1" si="2"/>
-        <v>-16</v>
+      <c r="G42" s="6">
+        <v>-113</v>
+      </c>
+      <c r="H42" s="6">
+        <v>55</v>
       </c>
       <c r="J42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(41,3,'Canada Central','Amérique du Nord','Canada','15','-16'),</v>
+        <f t="shared" si="0"/>
+        <v>(41,3,'Canada Central','Amérique du Nord','Canada','-113','55'),</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -2213,19 +2136,17 @@
         <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>88</v>
-      </c>
-      <c r="G43">
-        <f t="shared" ca="1" si="1"/>
-        <v>-22</v>
-      </c>
-      <c r="H43">
-        <f t="shared" ca="1" si="2"/>
-        <v>-13</v>
+        <v>30</v>
+      </c>
+      <c r="G43" s="6">
+        <v>-93.2</v>
+      </c>
+      <c r="H43" s="6">
+        <v>41.8</v>
       </c>
       <c r="J43" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(42,3,'US Gov Iowa','Amérique du Nord','etats-Unis','-22','-13'),</v>
+        <f t="shared" si="0"/>
+        <v>(42,3,'US Gov Iowa','Amérique du Nord','Etats-Unis','-93.2','41.8'),</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -2245,19 +2166,17 @@
         <v>27</v>
       </c>
       <c r="F44" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44">
-        <f t="shared" ca="1" si="1"/>
-        <v>162</v>
-      </c>
-      <c r="H44">
-        <f t="shared" ca="1" si="2"/>
-        <v>-18</v>
+        <v>30</v>
+      </c>
+      <c r="G44" s="6">
+        <v>-92</v>
+      </c>
+      <c r="H44" s="6">
+        <v>37</v>
       </c>
       <c r="J44" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(43,3,'Central US','Amérique du Nord','etats-Unis','162','-18'),</v>
+        <f t="shared" si="0"/>
+        <v>(43,3,'Central US','Amérique du Nord','Etats-Unis','-92','37'),</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -2277,19 +2196,17 @@
         <v>27</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
-      </c>
-      <c r="G45">
-        <f t="shared" ca="1" si="1"/>
-        <v>125</v>
-      </c>
-      <c r="H45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="G45" s="6">
+        <v>-93</v>
+      </c>
+      <c r="H45" s="6">
+        <v>47</v>
       </c>
       <c r="J45" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(44,3,'North Central US','Amérique du Nord','etats-Unis','125','0'),</v>
+        <f t="shared" si="0"/>
+        <v>(44,3,'North Central US','Amérique du Nord','Etats-Unis','-93','47'),</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2309,19 +2226,17 @@
         <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
-      </c>
-      <c r="G46">
-        <f t="shared" ca="1" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="H46">
-        <f t="shared" ca="1" si="2"/>
-        <v>-36</v>
+        <v>30</v>
+      </c>
+      <c r="G46" s="6">
+        <v>-78</v>
+      </c>
+      <c r="H46" s="6">
+        <v>37</v>
       </c>
       <c r="J46" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(45,3,'US DoD East','Amérique du Nord','etats-Unis','69','-36'),</v>
+        <f t="shared" si="0"/>
+        <v>(45,3,'US DoD East','Amérique du Nord','Etats-Unis','-78','37'),</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2341,19 +2256,17 @@
         <v>27</v>
       </c>
       <c r="F47" t="s">
-        <v>88</v>
-      </c>
-      <c r="G47">
-        <f t="shared" ca="1" si="1"/>
-        <v>-143</v>
-      </c>
-      <c r="H47">
-        <f t="shared" ca="1" si="2"/>
         <v>30</v>
       </c>
+      <c r="G47" s="6">
+        <v>-70</v>
+      </c>
+      <c r="H47" s="6">
+        <v>44</v>
+      </c>
       <c r="J47" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(46,3,'East US','Amérique du Nord','etats-Unis','-143','30'),</v>
+        <f t="shared" si="0"/>
+        <v>(46,3,'East US','Amérique du Nord','Etats-Unis','-70','44'),</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2373,19 +2286,17 @@
         <v>27</v>
       </c>
       <c r="F48" t="s">
-        <v>88</v>
-      </c>
-      <c r="G48">
-        <f t="shared" ca="1" si="1"/>
-        <v>-96</v>
-      </c>
-      <c r="H48">
-        <f t="shared" ca="1" si="2"/>
-        <v>-38</v>
+        <v>30</v>
+      </c>
+      <c r="G48" s="6">
+        <v>-72</v>
+      </c>
+      <c r="H48" s="6">
+        <v>42</v>
       </c>
       <c r="J48" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(47,3,'East US 2','Amérique du Nord','etats-Unis','-96','-38'),</v>
+        <f t="shared" si="0"/>
+        <v>(47,3,'East US 2','Amérique du Nord','Etats-Unis','-72','42'),</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2405,19 +2316,17 @@
         <v>27</v>
       </c>
       <c r="F49" t="s">
-        <v>88</v>
-      </c>
-      <c r="G49">
-        <f t="shared" ca="1" si="1"/>
-        <v>-100</v>
-      </c>
-      <c r="H49">
-        <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="G49" s="6">
+        <v>-77.8</v>
+      </c>
+      <c r="H49" s="6">
+        <v>37.700000000000003</v>
       </c>
       <c r="J49" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(48,3,'US Gov Virginia','Amérique du Nord','etats-Unis','-100','16'),</v>
+        <f t="shared" si="0"/>
+        <v>(48,3,'US Gov Virginia','Amérique du Nord','Etats-Unis','-77.8','37.7'),</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2437,19 +2346,17 @@
         <v>27</v>
       </c>
       <c r="F50" t="s">
-        <v>88</v>
-      </c>
-      <c r="G50">
-        <f t="shared" ca="1" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="H50">
-        <f t="shared" ca="1" si="2"/>
-        <v>-25</v>
+        <v>30</v>
+      </c>
+      <c r="G50" s="6">
+        <v>-100</v>
+      </c>
+      <c r="H50" s="6">
+        <v>38</v>
       </c>
       <c r="J50" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(49,3,'US DoD Central','Amérique du Nord','etats-Unis','40','-25'),</v>
+        <f t="shared" si="0"/>
+        <v>(49,3,'US DoD Central','Amérique du Nord','Etats-Unis','-100','38'),</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2469,19 +2376,17 @@
         <v>27</v>
       </c>
       <c r="F51" t="s">
-        <v>88</v>
-      </c>
-      <c r="G51">
-        <f t="shared" ca="1" si="1"/>
-        <v>-33</v>
-      </c>
-      <c r="H51">
-        <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+        <v>30</v>
+      </c>
+      <c r="G51" s="6">
+        <v>-119</v>
+      </c>
+      <c r="H51" s="6">
+        <v>39</v>
       </c>
       <c r="J51" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(50,3,'West US 2','Amérique du Nord','etats-Unis','-33','19'),</v>
+        <f t="shared" si="0"/>
+        <v>(50,3,'West US 2','Amérique du Nord','Etats-Unis','-119','39'),</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2501,19 +2406,17 @@
         <v>27</v>
       </c>
       <c r="F52" t="s">
-        <v>88</v>
-      </c>
-      <c r="G52">
-        <f t="shared" ca="1" si="1"/>
-        <v>-84</v>
-      </c>
-      <c r="H52">
-        <f t="shared" ca="1" si="2"/>
-        <v>-33</v>
+        <v>30</v>
+      </c>
+      <c r="G52" s="6">
+        <v>-109</v>
+      </c>
+      <c r="H52" s="6">
+        <v>40</v>
       </c>
       <c r="J52" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(51,3,'West Central US','Amérique du Nord','etats-Unis','-84','-33'),</v>
+        <f t="shared" si="0"/>
+        <v>(51,3,'West Central US','Amérique du Nord','Etats-Unis','-109','40'),</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2533,19 +2436,17 @@
         <v>27</v>
       </c>
       <c r="F53" t="s">
-        <v>88</v>
-      </c>
-      <c r="G53">
-        <f t="shared" ca="1" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="H53">
-        <f t="shared" ca="1" si="2"/>
-        <v>-50</v>
+        <v>30</v>
+      </c>
+      <c r="G53" s="6">
+        <v>-123</v>
+      </c>
+      <c r="H53" s="6">
+        <v>40</v>
       </c>
       <c r="J53" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(52,3,'West US','Amérique du Nord','etats-Unis','8','-50'),</v>
+        <f t="shared" si="0"/>
+        <v>(52,3,'West US','Amérique du Nord','Etats-Unis','-123','40'),</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2565,19 +2466,17 @@
         <v>27</v>
       </c>
       <c r="F54" t="s">
-        <v>88</v>
-      </c>
-      <c r="G54">
-        <f t="shared" ca="1" si="1"/>
-        <v>-44</v>
-      </c>
-      <c r="H54">
-        <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>30</v>
+      </c>
+      <c r="G54" s="6">
+        <v>-111.9</v>
+      </c>
+      <c r="H54" s="6">
+        <v>33.799999999999997</v>
       </c>
       <c r="J54" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(53,3,'US Gov Arizona','Amérique du Nord','etats-Unis','-44','14'),</v>
+        <f t="shared" si="0"/>
+        <v>(53,3,'US Gov Arizona','Amérique du Nord','Etats-Unis','-111.9','33.8'),</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2597,19 +2496,17 @@
         <v>27</v>
       </c>
       <c r="F55" t="s">
-        <v>88</v>
-      </c>
-      <c r="G55">
-        <f t="shared" ca="1" si="1"/>
-        <v>89</v>
-      </c>
-      <c r="H55">
-        <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="G55" s="6">
+        <v>-98</v>
+      </c>
+      <c r="H55" s="6">
+        <v>35</v>
       </c>
       <c r="J55" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(54,3,'South Central US','Amérique du Nord','etats-Unis','89','24'),</v>
+        <f t="shared" si="0"/>
+        <v>(54,3,'South Central US','Amérique du Nord','Etats-Unis','-98','35'),</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2629,18 +2526,18 @@
         <v>27</v>
       </c>
       <c r="F56" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="G56" s="6">
         <v>-97.8</v>
       </c>
-      <c r="H56">
-        <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+      <c r="H56" s="6">
+        <f t="shared" ref="H7:H70" ca="1" si="1">RANDBETWEEN(-50,50)</f>
+        <v>41</v>
       </c>
       <c r="J56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(55,3,'US Gov Texas','Amérique du Nord','etats-Unis','-97.8','34'),</v>
+        <v>(55,3,'US Gov Texas','Amérique du Nord','Etats-Unis','-97.8','41'),</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2662,17 +2559,15 @@
       <c r="F57" t="s">
         <v>68</v>
       </c>
-      <c r="G57">
-        <f t="shared" ca="1" si="1"/>
-        <v>-76</v>
-      </c>
-      <c r="H57">
-        <f t="shared" ca="1" si="2"/>
-        <v>-26</v>
+      <c r="G57" s="6">
+        <v>-53</v>
+      </c>
+      <c r="H57" s="6">
+        <v>-31</v>
       </c>
       <c r="J57" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(56,3,'Brazil South','Amérique du Sud','Brésil','-76','-26'),</v>
+        <f t="shared" si="0"/>
+        <v>(56,3,'Brazil South','Amérique du Sud','Brésil','-53','-31'),</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2686,25 +2581,23 @@
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E58" t="s">
         <v>25</v>
       </c>
       <c r="F58" t="s">
-        <v>103</v>
-      </c>
-      <c r="G58">
-        <f t="shared" ca="1" si="1"/>
-        <v>-81</v>
-      </c>
-      <c r="H58">
-        <f t="shared" ca="1" si="2"/>
-        <v>-41</v>
+        <v>102</v>
+      </c>
+      <c r="G58" s="6">
+        <v>6</v>
+      </c>
+      <c r="H58" s="6">
+        <v>60</v>
       </c>
       <c r="J58" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(57,3,'Norway West','Europe','Norvège','-81','-41'),</v>
+        <f t="shared" si="0"/>
+        <v>(57,3,'Norway West','Europe','Norvège','6','60'),</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2718,7 +2611,7 @@
         <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E59" t="s">
         <v>25</v>
@@ -2726,17 +2619,15 @@
       <c r="F59" t="s">
         <v>56</v>
       </c>
-      <c r="G59">
-        <f t="shared" ca="1" si="1"/>
-        <v>-70</v>
-      </c>
-      <c r="H59">
-        <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+      <c r="G59" s="6">
+        <v>5.4</v>
+      </c>
+      <c r="H59" s="6">
+        <v>52</v>
       </c>
       <c r="J59" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(58,3,'West Europe','Europe','Pays-Bas','-70','6'),</v>
+        <f t="shared" si="0"/>
+        <v>(58,3,'West Europe','Europe','Pays-Bas','5.4','52'),</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2750,7 +2641,7 @@
         <v>3</v>
       </c>
       <c r="D60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E60" t="s">
         <v>25</v>
@@ -2758,17 +2649,15 @@
       <c r="F60" t="s">
         <v>39</v>
       </c>
-      <c r="G60">
-        <f t="shared" ca="1" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="H60">
-        <f t="shared" ca="1" si="2"/>
-        <v>19</v>
+      <c r="G60" s="6">
+        <v>-1.8</v>
+      </c>
+      <c r="H60" s="6">
+        <v>51</v>
       </c>
       <c r="J60" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(59,3,'UK South','Europe','Grande-Bretagne','117','19'),</v>
+        <f t="shared" si="0"/>
+        <v>(59,3,'UK South','Europe','Grande-Bretagne','-1.8','51'),</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2782,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="D61" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E61" t="s">
         <v>25</v>
@@ -2790,17 +2679,15 @@
       <c r="F61" t="s">
         <v>38</v>
       </c>
-      <c r="G61">
-        <f t="shared" ca="1" si="1"/>
-        <v>-98</v>
-      </c>
-      <c r="H61">
-        <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+      <c r="G61" s="6">
+        <v>-9</v>
+      </c>
+      <c r="H61" s="6">
+        <v>52</v>
       </c>
       <c r="J61" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(60,3,'North Europe','Europe','Irlande','-98','9'),</v>
+        <f t="shared" si="0"/>
+        <v>(60,3,'North Europe','Europe','Irlande','-9','52'),</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2814,7 +2701,7 @@
         <v>3</v>
       </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E62" t="s">
         <v>25</v>
@@ -2822,17 +2709,15 @@
       <c r="F62" t="s">
         <v>39</v>
       </c>
-      <c r="G62">
-        <f t="shared" ca="1" si="1"/>
-        <v>-163</v>
-      </c>
-      <c r="H62">
-        <f t="shared" ca="1" si="2"/>
-        <v>-26</v>
+      <c r="G62" s="6">
+        <v>-4</v>
+      </c>
+      <c r="H62" s="6">
+        <v>52</v>
       </c>
       <c r="J62" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(61,3,'UK West','Europe','Grande-Bretagne','-163','-26'),</v>
+        <f t="shared" si="0"/>
+        <v>(61,3,'UK West','Europe','Grande-Bretagne','-4','52'),</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2846,7 +2731,7 @@
         <v>3</v>
       </c>
       <c r="D63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E63" t="s">
         <v>25</v>
@@ -2854,17 +2739,15 @@
       <c r="F63" t="s">
         <v>40</v>
       </c>
-      <c r="G63">
-        <f t="shared" ca="1" si="1"/>
-        <v>-46</v>
-      </c>
-      <c r="H63">
-        <f t="shared" ca="1" si="2"/>
-        <v>-11</v>
+      <c r="G63" s="6">
+        <v>2</v>
+      </c>
+      <c r="H63" s="6">
+        <v>47</v>
       </c>
       <c r="J63" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(62,3,'France Central','Europe','France','-46','-11'),</v>
+        <f t="shared" si="0"/>
+        <v>(62,3,'France Central','Europe','France','2','47'),</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2878,7 +2761,7 @@
         <v>3</v>
       </c>
       <c r="D64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E64" t="s">
         <v>25</v>
@@ -2886,17 +2769,15 @@
       <c r="F64" t="s">
         <v>40</v>
       </c>
-      <c r="G64">
-        <f t="shared" ca="1" si="1"/>
-        <v>-18</v>
-      </c>
-      <c r="H64">
-        <f t="shared" ca="1" si="2"/>
-        <v>-11</v>
+      <c r="G64" s="6">
+        <v>3</v>
+      </c>
+      <c r="H64" s="6">
+        <v>44</v>
       </c>
       <c r="J64" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(63,3,'France South','Europe','France','-18','-11'),</v>
+        <f t="shared" si="0"/>
+        <v>(63,3,'France South','Europe','France','3','44'),</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2910,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="D65" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E65" t="s">
         <v>25</v>
@@ -2918,17 +2799,15 @@
       <c r="F65" t="s">
         <v>69</v>
       </c>
-      <c r="G65">
-        <f t="shared" ca="1" si="1"/>
-        <v>111</v>
-      </c>
-      <c r="H65">
-        <f t="shared" ca="1" si="2"/>
-        <v>-3</v>
+      <c r="G65" s="6">
+        <v>7</v>
+      </c>
+      <c r="H65" s="6">
+        <v>47</v>
       </c>
       <c r="J65" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(64,3,'Switzerland West','Europe','Suisse','111','-3'),</v>
+        <f t="shared" si="0"/>
+        <v>(64,3,'Switzerland West','Europe','Suisse','7','47'),</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2942,7 +2821,7 @@
         <v>3</v>
       </c>
       <c r="D66" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E66" t="s">
         <v>25</v>
@@ -2950,17 +2829,15 @@
       <c r="F66" t="s">
         <v>69</v>
       </c>
-      <c r="G66">
-        <f t="shared" ca="1" si="1"/>
-        <v>-105</v>
-      </c>
-      <c r="H66">
-        <f t="shared" ca="1" si="2"/>
-        <v>-50</v>
+      <c r="G66" s="6">
+        <v>8</v>
+      </c>
+      <c r="H66" s="6">
+        <v>47</v>
       </c>
       <c r="J66" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>(65,3,'Switzerland North','Europe','Suisse','-105','-50'),</v>
+        <f t="shared" si="0"/>
+        <v>(65,3,'Switzerland North','Europe','Suisse','8','47'),</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2974,7 +2851,7 @@
         <v>3</v>
       </c>
       <c r="D67" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E67" t="s">
         <v>25</v>
@@ -2982,17 +2859,15 @@
       <c r="F67" t="s">
         <v>37</v>
       </c>
-      <c r="G67">
-        <f t="shared" ca="1" si="1"/>
-        <v>-151</v>
-      </c>
-      <c r="H67">
-        <f t="shared" ca="1" si="2"/>
-        <v>-7</v>
+      <c r="G67" s="6">
+        <v>11</v>
+      </c>
+      <c r="H67" s="6">
+        <v>52</v>
       </c>
       <c r="J67" t="str">
-        <f t="shared" ref="J67:J92" ca="1" si="3">CONCATENATE("(",B67,",",C67,",'",D67,"','",E67,"','",F67,"','",G67,"','",H67,"'),")</f>
-        <v>(66,3,'Germany Central','Europe','Allemagne','-151','-7'),</v>
+        <f t="shared" ref="J67:J92" si="2">CONCATENATE("(",B67,",",C67,",'",D67,"','",E67,"','",F67,"','",G67,"','",H67,"'),")</f>
+        <v>(66,3,'Germany Central','Europe','Allemagne','11','52'),</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -3006,7 +2881,7 @@
         <v>3</v>
       </c>
       <c r="D68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E68" t="s">
         <v>25</v>
@@ -3014,17 +2889,15 @@
       <c r="F68" t="s">
         <v>37</v>
       </c>
-      <c r="G68">
-        <f t="shared" ca="1" si="1"/>
-        <v>180</v>
-      </c>
-      <c r="H68">
-        <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+      <c r="G68" s="6">
+        <v>8</v>
+      </c>
+      <c r="H68" s="6">
+        <v>53</v>
       </c>
       <c r="J68" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(67,3,'Germany Northeast','Europe','Allemagne','180','14'),</v>
+        <f t="shared" si="2"/>
+        <v>(67,3,'Germany Northeast','Europe','Allemagne','8','53'),</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -3038,7 +2911,7 @@
         <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E69" t="s">
         <v>25</v>
@@ -3046,17 +2919,15 @@
       <c r="F69" t="s">
         <v>37</v>
       </c>
-      <c r="G69">
-        <f t="shared" ca="1" si="1"/>
-        <v>-94</v>
-      </c>
-      <c r="H69">
-        <f t="shared" ca="1" si="2"/>
-        <v>-16</v>
+      <c r="G69" s="6">
+        <v>11</v>
+      </c>
+      <c r="H69" s="6">
+        <v>54</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(68,3,'Germany North','Europe','Allemagne','-94','-16'),</v>
+        <f t="shared" si="2"/>
+        <v>(68,3,'Germany North','Europe','Allemagne','11','54'),</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -3070,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="D70" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E70" t="s">
         <v>25</v>
@@ -3078,17 +2949,15 @@
       <c r="F70" t="s">
         <v>37</v>
       </c>
-      <c r="G70">
-        <f t="shared" ca="1" si="1"/>
-        <v>129</v>
-      </c>
-      <c r="H70">
-        <f t="shared" ca="1" si="2"/>
-        <v>-46</v>
+      <c r="G70" s="6">
+        <v>9</v>
+      </c>
+      <c r="H70" s="6">
+        <v>49</v>
       </c>
       <c r="J70" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(69,3,'Germany West Central','Europe','Allemagne','129','-46'),</v>
+        <f t="shared" si="2"/>
+        <v>(69,3,'Germany West Central','Europe','Allemagne','9','49'),</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -3102,25 +2971,23 @@
         <v>3</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E71" t="s">
         <v>25</v>
       </c>
       <c r="F71" t="s">
-        <v>103</v>
-      </c>
-      <c r="G71">
-        <f t="shared" ref="G71:G92" ca="1" si="4">RANDBETWEEN(-180,180)</f>
-        <v>-97</v>
-      </c>
-      <c r="H71">
-        <f t="shared" ref="H71:H92" ca="1" si="5">RANDBETWEEN(-50,50)</f>
-        <v>-42</v>
+        <v>102</v>
+      </c>
+      <c r="G71" s="6">
+        <v>11</v>
+      </c>
+      <c r="H71" s="6">
+        <v>60</v>
       </c>
       <c r="J71" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(70,3,'Norway East','Europe','Norvège','-97','-42'),</v>
+        <f t="shared" si="2"/>
+        <v>(70,3,'Norway East','Europe','Norvège','11','60'),</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -3134,25 +3001,23 @@
         <v>3</v>
       </c>
       <c r="D72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E72" t="s">
+        <v>105</v>
+      </c>
+      <c r="F72" t="s">
         <v>106</v>
       </c>
-      <c r="F72" t="s">
-        <v>107</v>
-      </c>
-      <c r="G72">
-        <f t="shared" ca="1" si="4"/>
-        <v>69</v>
-      </c>
-      <c r="H72">
-        <f t="shared" ca="1" si="5"/>
-        <v>-38</v>
+      <c r="G72" s="6">
+        <v>19</v>
+      </c>
+      <c r="H72" s="6">
+        <v>-33</v>
       </c>
       <c r="J72" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(71,3,'South Africa West','Afrique','Afrique du Sud','69','-38'),</v>
+        <f t="shared" si="2"/>
+        <v>(71,3,'South Africa West','Afrique','Afrique du Sud','19','-33'),</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -3166,25 +3031,23 @@
         <v>3</v>
       </c>
       <c r="D73" t="s">
+        <v>104</v>
+      </c>
+      <c r="E73" t="s">
         <v>105</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>106</v>
       </c>
-      <c r="F73" t="s">
-        <v>107</v>
-      </c>
-      <c r="G73">
-        <f t="shared" ca="1" si="4"/>
-        <v>23</v>
-      </c>
-      <c r="H73">
-        <f t="shared" ca="1" si="5"/>
-        <v>15</v>
+      <c r="G73" s="6">
+        <v>28</v>
+      </c>
+      <c r="H73" s="6">
+        <v>-26</v>
       </c>
       <c r="J73" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(72,3,'South Africa North','Afrique','Afrique du Sud','23','15'),</v>
+        <f t="shared" si="2"/>
+        <v>(72,3,'South Africa North','Afrique','Afrique du Sud','28','-26'),</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -3198,25 +3061,23 @@
         <v>3</v>
       </c>
       <c r="D74" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E74" t="s">
         <v>28</v>
       </c>
       <c r="F74" t="s">
-        <v>127</v>
-      </c>
-      <c r="G74">
-        <f t="shared" ca="1" si="4"/>
-        <v>-146</v>
-      </c>
-      <c r="H74">
-        <f t="shared" ca="1" si="5"/>
-        <v>28</v>
+        <v>126</v>
+      </c>
+      <c r="G74" s="6">
+        <v>55</v>
+      </c>
+      <c r="H74" s="6">
+        <v>24</v>
       </c>
       <c r="J74" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(73,3,'UAE Central','Asie-Pacifique','Emirats Arabes Unis','-146','28'),</v>
+        <f t="shared" si="2"/>
+        <v>(73,3,'UAE Central','Asie-Pacifique','Emirats Arabes Unis','55','24'),</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -3230,25 +3091,23 @@
         <v>3</v>
       </c>
       <c r="D75" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E75" t="s">
         <v>28</v>
       </c>
       <c r="F75" t="s">
-        <v>127</v>
-      </c>
-      <c r="G75">
-        <f t="shared" ca="1" si="4"/>
-        <v>178</v>
-      </c>
-      <c r="H75">
-        <f t="shared" ca="1" si="5"/>
-        <v>30</v>
+        <v>126</v>
+      </c>
+      <c r="G75" s="6">
+        <v>56</v>
+      </c>
+      <c r="H75" s="6">
+        <v>25</v>
       </c>
       <c r="J75" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(74,3,'UAE North','Asie-Pacifique','Emirats Arabes Unis','178','30'),</v>
+        <f t="shared" si="2"/>
+        <v>(74,3,'UAE North','Asie-Pacifique','Emirats Arabes Unis','56','25'),</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -3262,7 +3121,7 @@
         <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E76" t="s">
         <v>28</v>
@@ -3270,17 +3129,15 @@
       <c r="F76" t="s">
         <v>33</v>
       </c>
-      <c r="G76">
-        <f t="shared" ca="1" si="4"/>
-        <v>-171</v>
-      </c>
-      <c r="H76">
-        <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+      <c r="G76" s="6">
+        <v>74</v>
+      </c>
+      <c r="H76" s="6">
+        <v>17</v>
       </c>
       <c r="J76" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(75,3,'West India','Asie-Pacifique','Inde','-171','19'),</v>
+        <f t="shared" si="2"/>
+        <v>(75,3,'West India','Asie-Pacifique','Inde','74','17'),</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -3294,7 +3151,7 @@
         <v>3</v>
       </c>
       <c r="D77" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E77" t="s">
         <v>28</v>
@@ -3302,17 +3159,15 @@
       <c r="F77" t="s">
         <v>33</v>
       </c>
-      <c r="G77">
-        <f t="shared" ca="1" si="4"/>
-        <v>-64</v>
-      </c>
-      <c r="H77">
-        <f t="shared" ca="1" si="5"/>
-        <v>-10</v>
+      <c r="G77" s="6">
+        <v>78</v>
+      </c>
+      <c r="H77" s="6">
+        <v>20</v>
       </c>
       <c r="J77" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(76,3,'Central India','Asie-Pacifique','Inde','-64','-10'),</v>
+        <f t="shared" si="2"/>
+        <v>(76,3,'Central India','Asie-Pacifique','Inde','78','20'),</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -3326,7 +3181,7 @@
         <v>3</v>
       </c>
       <c r="D78" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E78" t="s">
         <v>28</v>
@@ -3334,17 +3189,15 @@
       <c r="F78" t="s">
         <v>33</v>
       </c>
-      <c r="G78">
-        <f t="shared" ca="1" si="4"/>
-        <v>116</v>
-      </c>
-      <c r="H78">
-        <f t="shared" ca="1" si="5"/>
-        <v>-16</v>
+      <c r="G78" s="6">
+        <v>77</v>
+      </c>
+      <c r="H78" s="6">
+        <v>11</v>
       </c>
       <c r="J78" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(77,3,'South India','Asie-Pacifique','Inde','116','-16'),</v>
+        <f t="shared" si="2"/>
+        <v>(77,3,'South India','Asie-Pacifique','Inde','77','11'),</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -3358,7 +3211,7 @@
         <v>3</v>
       </c>
       <c r="D79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E79" t="s">
         <v>28</v>
@@ -3366,17 +3219,15 @@
       <c r="F79" t="s">
         <v>65</v>
       </c>
-      <c r="G79">
-        <f t="shared" ca="1" si="4"/>
-        <v>105</v>
-      </c>
-      <c r="H79">
-        <f t="shared" ca="1" si="5"/>
-        <v>-25</v>
+      <c r="G79" s="6">
+        <v>103.7</v>
+      </c>
+      <c r="H79" s="6">
+        <v>1.4</v>
       </c>
       <c r="J79" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(78,3,'Southeast Asia','Asie-Pacifique','Singapour','105','-25'),</v>
+        <f t="shared" si="2"/>
+        <v>(78,3,'Southeast Asia','Asie-Pacifique','Singapour','103.7','1.4'),</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -3390,25 +3241,23 @@
         <v>3</v>
       </c>
       <c r="D80" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E80" t="s">
         <v>28</v>
       </c>
       <c r="F80" t="s">
-        <v>128</v>
-      </c>
-      <c r="G80">
-        <f t="shared" ca="1" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="H80">
-        <f t="shared" ca="1" si="5"/>
-        <v>-3</v>
+        <v>127</v>
+      </c>
+      <c r="G80" s="6">
+        <v>115</v>
+      </c>
+      <c r="H80" s="6">
+        <v>39</v>
       </c>
       <c r="J80" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(79,3,'China North','Asie-Pacifique','Chine','7','-3'),</v>
+        <f t="shared" si="2"/>
+        <v>(79,3,'China North','Asie-Pacifique','Chine','115','39'),</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -3422,25 +3271,23 @@
         <v>3</v>
       </c>
       <c r="D81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E81" t="s">
         <v>28</v>
       </c>
       <c r="F81" t="s">
-        <v>128</v>
-      </c>
-      <c r="G81">
-        <f t="shared" ca="1" si="4"/>
-        <v>5</v>
-      </c>
-      <c r="H81">
-        <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>127</v>
+      </c>
+      <c r="G81" s="6">
+        <v>118</v>
+      </c>
+      <c r="H81" s="6">
+        <v>37</v>
       </c>
       <c r="J81" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(80,3,'China North 2','Asie-Pacifique','Chine','5','0'),</v>
+        <f t="shared" si="2"/>
+        <v>(80,3,'China North 2','Asie-Pacifique','Chine','118','37'),</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -3454,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="D82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E82" t="s">
         <v>28</v>
@@ -3462,17 +3309,15 @@
       <c r="F82" t="s">
         <v>35</v>
       </c>
-      <c r="G82">
-        <f t="shared" ca="1" si="4"/>
-        <v>99</v>
-      </c>
-      <c r="H82">
-        <f t="shared" ca="1" si="5"/>
-        <v>-36</v>
+      <c r="G82" s="6">
+        <v>128</v>
+      </c>
+      <c r="H82" s="6">
+        <v>36</v>
       </c>
       <c r="J82" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(81,3,'Korea Central','Asie-Pacifique','Corée du Sud','99','-36'),</v>
+        <f t="shared" si="2"/>
+        <v>(81,3,'Korea Central','Asie-Pacifique','Corée du Sud','128','36'),</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -3486,7 +3331,7 @@
         <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E83" t="s">
         <v>28</v>
@@ -3494,17 +3339,15 @@
       <c r="F83" t="s">
         <v>35</v>
       </c>
-      <c r="G83">
-        <f t="shared" ca="1" si="4"/>
-        <v>-79</v>
-      </c>
-      <c r="H83">
-        <f t="shared" ca="1" si="5"/>
+      <c r="G83" s="6">
+        <v>127</v>
+      </c>
+      <c r="H83" s="6">
         <v>35</v>
       </c>
       <c r="J83" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(82,3,'Korea South','Asie-Pacifique','Corée du Sud','-79','35'),</v>
+        <f t="shared" si="2"/>
+        <v>(82,3,'Korea South','Asie-Pacifique','Corée du Sud','127','35'),</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -3518,25 +3361,23 @@
         <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E84" t="s">
         <v>28</v>
       </c>
       <c r="F84" t="s">
-        <v>128</v>
-      </c>
-      <c r="G84">
-        <f t="shared" ca="1" si="4"/>
-        <v>-40</v>
-      </c>
-      <c r="H84">
-        <f t="shared" ca="1" si="5"/>
-        <v>-10</v>
+        <v>127</v>
+      </c>
+      <c r="G84" s="6">
+        <v>121</v>
+      </c>
+      <c r="H84" s="6">
+        <v>30</v>
       </c>
       <c r="J84" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(83,3,'China East','Asie-Pacifique','Chine','-40','-10'),</v>
+        <f t="shared" si="2"/>
+        <v>(83,3,'China East','Asie-Pacifique','Chine','121','30'),</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -3550,25 +3391,23 @@
         <v>3</v>
       </c>
       <c r="D85" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E85" t="s">
         <v>28</v>
       </c>
       <c r="F85" t="s">
-        <v>128</v>
-      </c>
-      <c r="G85">
-        <f t="shared" ca="1" si="4"/>
-        <v>-104</v>
-      </c>
-      <c r="H85">
-        <f t="shared" ca="1" si="5"/>
-        <v>-25</v>
+        <v>127</v>
+      </c>
+      <c r="G85" s="6">
+        <v>120</v>
+      </c>
+      <c r="H85" s="6">
+        <v>28</v>
       </c>
       <c r="J85" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(84,3,'China East 2','Asie-Pacifique','Chine','-104','-25'),</v>
+        <f t="shared" si="2"/>
+        <v>(84,3,'China East 2','Asie-Pacifique','Chine','120','28'),</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -3582,25 +3421,23 @@
         <v>3</v>
       </c>
       <c r="D86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E86" t="s">
         <v>28</v>
       </c>
       <c r="F86" t="s">
-        <v>128</v>
-      </c>
-      <c r="G86">
-        <f t="shared" ca="1" si="4"/>
-        <v>-97</v>
-      </c>
-      <c r="H86">
-        <f t="shared" ca="1" si="5"/>
-        <v>-10</v>
+        <v>127</v>
+      </c>
+      <c r="G86" s="6">
+        <v>115</v>
+      </c>
+      <c r="H86" s="6">
+        <v>23</v>
       </c>
       <c r="J86" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(85,3,'East Asia','Asie-Pacifique','Chine','-97','-10'),</v>
+        <f t="shared" si="2"/>
+        <v>(85,3,'East Asia','Asie-Pacifique','Chine','115','23'),</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -3614,7 +3451,7 @@
         <v>3</v>
       </c>
       <c r="D87" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E87" t="s">
         <v>28</v>
@@ -3622,17 +3459,15 @@
       <c r="F87" t="s">
         <v>34</v>
       </c>
-      <c r="G87">
-        <f t="shared" ca="1" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="H87">
-        <f t="shared" ca="1" si="5"/>
-        <v>44</v>
+      <c r="G87" s="6">
+        <v>140</v>
+      </c>
+      <c r="H87" s="6">
+        <v>37</v>
       </c>
       <c r="J87" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(86,3,'Japan East','Asie-Pacifique','Japon','18','44'),</v>
+        <f t="shared" si="2"/>
+        <v>(86,3,'Japan East','Asie-Pacifique','Japon','140','37'),</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -3646,7 +3481,7 @@
         <v>3</v>
       </c>
       <c r="D88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E88" t="s">
         <v>28</v>
@@ -3654,17 +3489,15 @@
       <c r="F88" t="s">
         <v>34</v>
       </c>
-      <c r="G88">
-        <f t="shared" ca="1" si="4"/>
-        <v>-45</v>
-      </c>
-      <c r="H88">
-        <f t="shared" ca="1" si="5"/>
-        <v>19</v>
+      <c r="G88" s="6">
+        <v>131</v>
+      </c>
+      <c r="H88" s="6">
+        <v>33</v>
       </c>
       <c r="J88" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(87,3,'Japan West','Asie-Pacifique','Japon','-45','19'),</v>
+        <f t="shared" si="2"/>
+        <v>(87,3,'Japan West','Asie-Pacifique','Japon','131','33'),</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -3678,7 +3511,7 @@
         <v>3</v>
       </c>
       <c r="D89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E89" t="s">
         <v>28</v>
@@ -3686,17 +3519,15 @@
       <c r="F89" t="s">
         <v>36</v>
       </c>
-      <c r="G89">
-        <f t="shared" ca="1" si="4"/>
-        <v>-40</v>
-      </c>
-      <c r="H89">
-        <f t="shared" ca="1" si="5"/>
-        <v>45</v>
+      <c r="G89" s="6">
+        <v>151</v>
+      </c>
+      <c r="H89" s="6">
+        <v>-31</v>
       </c>
       <c r="J89" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(88,3,'Australia East','Asie-Pacifique','Australie','-40','45'),</v>
+        <f t="shared" si="2"/>
+        <v>(88,3,'Australia East','Asie-Pacifique','Australie','151','-31'),</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -3710,7 +3541,7 @@
         <v>3</v>
       </c>
       <c r="D90" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E90" t="s">
         <v>28</v>
@@ -3718,17 +3549,15 @@
       <c r="F90" t="s">
         <v>36</v>
       </c>
-      <c r="G90">
-        <f t="shared" ca="1" si="4"/>
-        <v>-137</v>
-      </c>
-      <c r="H90">
-        <f t="shared" ca="1" si="5"/>
-        <v>-45</v>
+      <c r="G90" s="6">
+        <v>148</v>
+      </c>
+      <c r="H90" s="6">
+        <v>-37</v>
       </c>
       <c r="J90" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(89,3,'Australia Southeast','Asie-Pacifique','Australie','-137','-45'),</v>
+        <f t="shared" si="2"/>
+        <v>(89,3,'Australia Southeast','Asie-Pacifique','Australie','148','-37'),</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -3742,7 +3571,7 @@
         <v>3</v>
       </c>
       <c r="D91" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E91" t="s">
         <v>28</v>
@@ -3750,17 +3579,15 @@
       <c r="F91" t="s">
         <v>36</v>
       </c>
-      <c r="G91">
-        <f t="shared" ca="1" si="4"/>
-        <v>119</v>
-      </c>
-      <c r="H91">
-        <f t="shared" ca="1" si="5"/>
-        <v>-47</v>
+      <c r="G91" s="6">
+        <v>132</v>
+      </c>
+      <c r="H91" s="6">
+        <v>-29</v>
       </c>
       <c r="J91" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(90,3,'Australia Central','Asie-Pacifique','Australie','119','-47'),</v>
+        <f t="shared" si="2"/>
+        <v>(90,3,'Australia Central','Asie-Pacifique','Australie','132','-29'),</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3774,7 +3601,7 @@
         <v>3</v>
       </c>
       <c r="D92" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E92" t="s">
         <v>28</v>
@@ -3782,17 +3609,15 @@
       <c r="F92" t="s">
         <v>36</v>
       </c>
-      <c r="G92">
-        <f t="shared" ca="1" si="4"/>
-        <v>125</v>
-      </c>
-      <c r="H92">
-        <f t="shared" ca="1" si="5"/>
-        <v>32</v>
+      <c r="G92" s="6">
+        <v>133</v>
+      </c>
+      <c r="H92" s="6">
+        <v>-24</v>
       </c>
       <c r="J92" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v>(91,3,'Australia Central 2','Asie-Pacifique','Australie','125','32'),</v>
+        <f t="shared" si="2"/>
+        <v>(91,3,'Australia Central 2','Asie-Pacifique','Australie','133','-24'),</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change Format & Country model, add indicators for Country & Data Providers
</commit_message>
<xml_diff>
--- a/data/db/data providers.xlsx
+++ b/data/db/data providers.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BA10EA1-9449-487E-858B-756D14833560}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAFF2AF-3B1D-45BD-AE03-FE0C2B7623B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="data providers" sheetId="3" r:id="rId1"/>
+    <sheet name="data centers" sheetId="1" r:id="rId2"/>
+    <sheet name="countries" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$J$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'data centers'!$A$1:$K$92</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="150">
   <si>
     <t>Amazon</t>
   </si>
@@ -430,13 +431,70 @@
   </si>
   <si>
     <t>latitude</t>
+  </si>
+  <si>
+    <t>Accounts Receivable Turnover Ratio</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Operating Cash-Flow Ratio</t>
+  </si>
+  <si>
+    <t>Current Ratio</t>
+  </si>
+  <si>
+    <t>Quick ratio</t>
+  </si>
+  <si>
+    <t>Return on assets</t>
+  </si>
+  <si>
+    <t>Pretax Net Profit Margin</t>
+  </si>
+  <si>
+    <t>Inventory Turnover</t>
+  </si>
+  <si>
+    <t>Fragile State Index</t>
+  </si>
+  <si>
+    <t>ICT Development Index</t>
+  </si>
+  <si>
+    <t>Human Development Index</t>
+  </si>
+  <si>
+    <t>ind_current_ratio</t>
+  </si>
+  <si>
+    <t>ind_quick_ratio</t>
+  </si>
+  <si>
+    <t>ind_return_on_assets</t>
+  </si>
+  <si>
+    <t>ind_accounts_receivable_turnover_ratio</t>
+  </si>
+  <si>
+    <t>ind_operating_cash_flow_ratio</t>
+  </si>
+  <si>
+    <t>ind_pretax_net_profit_margin</t>
+  </si>
+  <si>
+    <t>ind_inventory_turnover</t>
+  </si>
+  <si>
+    <t>country_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -446,24 +504,13 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF202124"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF37474F"/>
-      <name val="Roboto Mono"/>
-      <family val="3"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -472,18 +519,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -491,48 +532,16 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFDADCE0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFDADCE0"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFDADCE0"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,14 +855,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC19A3D-01C7-400F-ABF6-368E3B90A145}">
-  <dimension ref="A1:J92"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87765F3-A5A8-4725-B7FA-B36A7F3DBCF9}">
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2">
+        <v>3.35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2.5258446049252656</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.2656767710327763</v>
+      </c>
+      <c r="E2" s="3">
+        <v>3.2274304815939372</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3">
+        <v>3.37</v>
+      </c>
+      <c r="C3" s="3">
+        <v>5.3877467853265566</v>
+      </c>
+      <c r="D3" s="3">
+        <v>5.9730565161395015</v>
+      </c>
+      <c r="E3" s="3">
+        <v>6.2194217786127517</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.97817722360945869</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.80474144081162668</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.78470492698023953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.13519999999999999</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.37083480085750264</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.46260359609158275</v>
+      </c>
+      <c r="E5" s="3">
+        <v>7.1202715190883836E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3.9699999999999999E-2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.1388681822999143E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.57441374826137359</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.60754446660634231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.2122</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.55513650686658345</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.95349319709774616</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.51436795265188862</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8">
+        <v>68.28</v>
+      </c>
+      <c r="C8" s="3">
+        <v>44.675157795850659</v>
+      </c>
+      <c r="D8" s="3">
+        <v>57.696169051922404</v>
+      </c>
+      <c r="E8" s="3">
+        <v>43.583337224668419</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3.27</v>
+      </c>
+      <c r="D13" s="3">
+        <v>5.97</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.46</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I13" s="3">
+        <v>57.7</v>
+      </c>
+      <c r="J13" t="str">
+        <f>CONCATENATE("(",A13,",'",B13,"','",C13,"','",D13,"','",E13,"','",F13,"','",G13,"','",H13,"','",I13,"'),")</f>
+        <v>(1,'Amazon','3.27','5.97','0.8','0.46','0.57','0.95','57.7'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14">
+        <v>3.35</v>
+      </c>
+      <c r="D14">
+        <v>3.37</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.04</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="I14">
+        <v>68.28</v>
+      </c>
+      <c r="J14" t="str">
+        <f t="shared" ref="J14:J15" si="0">CONCATENATE("(",A14,",'",B14,"','",C14,"','",D14,"','",E14,"','",F14,"','",G14,"','",H14,"','",I14,"'),")</f>
+        <v>(2,'Google','3.35','3.37','0.14','0.14','0.04','0.21','68.28'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="D15" s="3">
+        <v>5.39</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.98</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="I15" s="3">
+        <v>44.68</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Microsoft','2.53','5.39','0.98','0.37','0.03','0.56','44.68'),</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC19A3D-01C7-400F-ABF6-368E3B90A145}">
+  <dimension ref="A1:K92"/>
+  <sheetViews>
+    <sheetView topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
@@ -861,9 +1162,10 @@
     <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>128</v>
       </c>
@@ -883,13 +1185,16 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" t="s">
         <v>129</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -908,18 +1213,22 @@
       <c r="F2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2">
+        <f>VLOOKUP(F2,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H2" s="1">
         <v>-82.9</v>
       </c>
-      <c r="H2" s="6">
+      <c r="I2" s="1">
         <v>39.9</v>
       </c>
-      <c r="J2" t="str">
-        <f>CONCATENATE("(",B2,",",C2,",'",D2,"','",E2,"','",F2,"','",G2,"','",H2,"'),")</f>
-        <v>(1,1,'US East (Ohio)','Amérique du Nord','Etats-Unis','-82.9','39.9'),</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" t="str">
+        <f>CONCATENATE("(",B2,",",C2,",'",D2,"',",G2,",'",H2,"','",I2,"'),")</f>
+        <v>(1,1,'US East (Ohio)',11,'-82.9','39.9'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -938,18 +1247,22 @@
       <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3">
+        <f>VLOOKUP(F3,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H3" s="1">
         <v>-77.400000000000006</v>
       </c>
-      <c r="H3" s="6">
+      <c r="I3" s="1">
         <v>37.5</v>
       </c>
-      <c r="J3" t="str">
-        <f t="shared" ref="J3:J66" si="0">CONCATENATE("(",B3,",",C3,",'",D3,"','",E3,"','",F3,"','",G3,"','",H3,"'),")</f>
-        <v>(2,1,'US East (N. Virginia)','Amérique du Nord','Etats-Unis','-77.4','37.5'),</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K66" si="0">CONCATENATE("(",B3,",",C3,",'",D3,"',",G3,",'",H3,"','",I3,"'),")</f>
+        <v>(2,1,'US East (N. Virginia)',11,'-77.4','37.5'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -968,18 +1281,22 @@
       <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4">
+        <f>VLOOKUP(F4,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H4" s="1">
         <v>-121.5</v>
       </c>
-      <c r="H4" s="6">
+      <c r="I4" s="1">
         <v>38.6</v>
       </c>
-      <c r="J4" t="str">
-        <f t="shared" si="0"/>
-        <v>(3,1,'US West (N. California)','Amérique du Nord','Etats-Unis','-121.5','38.6'),</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,1,'US West (N. California)',11,'-121.5','38.6'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -998,18 +1315,22 @@
       <c r="F5" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5">
+        <f>VLOOKUP(F5,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H5" s="1">
         <v>-122.7</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="1">
         <v>45.5</v>
       </c>
-      <c r="J5" t="str">
-        <f t="shared" si="0"/>
-        <v>(4,1,'US West (Oregon)','Amérique du Nord','Etats-Unis','-122.7','45.5'),</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,1,'US West (Oregon)',11,'-122.7','45.5'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1028,18 +1349,22 @@
       <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6">
+        <f>VLOOKUP(F6,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="H6" s="1">
         <v>114</v>
       </c>
-      <c r="H6" s="6">
+      <c r="I6" s="1">
         <v>22</v>
       </c>
-      <c r="J6" t="str">
-        <f t="shared" si="0"/>
-        <v>(5,1,'Asia Pacific (Hong Kong)','Asie-Pacifique','Hong Kong','114','22'),</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,1,'Asia Pacific (Hong Kong)',15,'114','22'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1058,18 +1383,22 @@
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7">
+        <f>VLOOKUP(F7,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="H7" s="1">
         <v>73</v>
       </c>
-      <c r="H7" s="6">
+      <c r="I7" s="1">
         <v>19</v>
       </c>
-      <c r="J7" t="str">
-        <f t="shared" si="0"/>
-        <v>(6,1,'Asia Pacific (Mumbai)','Asie-Pacifique','Inde','73','19'),</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="K7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,1,'Asia Pacific (Mumbai)',16,'73','19'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1088,18 +1417,22 @@
       <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8">
+        <f>VLOOKUP(F8,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H8" s="1">
         <v>136</v>
       </c>
-      <c r="H8" s="6">
+      <c r="I8" s="1">
         <v>35</v>
       </c>
-      <c r="J8" t="str">
-        <f t="shared" si="0"/>
-        <v>(7,1,'Asia Pacific (Osaka-Local)','Asie-Pacifique','Japon','136','35'),</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="K8" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,1,'Asia Pacific (Osaka-Local)',18,'136','35'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1118,18 +1451,22 @@
       <c r="F9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9">
+        <f>VLOOKUP(F9,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="H9" s="1">
         <v>127</v>
       </c>
-      <c r="H9" s="6">
+      <c r="I9" s="1">
         <v>37</v>
       </c>
-      <c r="J9" t="str">
-        <f t="shared" si="0"/>
-        <v>(8,1,'Asia Pacific (Seoul)','Asie-Pacifique','Corée du Sud','127','37'),</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="K9" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,1,'Asia Pacific (Seoul)',9,'127','37'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1148,18 +1485,22 @@
       <c r="F10" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10">
+        <f>VLOOKUP(F10,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="H10" s="1">
         <v>103.7</v>
       </c>
-      <c r="H10" s="6">
+      <c r="I10" s="1">
         <v>1.4</v>
       </c>
-      <c r="J10" t="str">
-        <f t="shared" si="0"/>
-        <v>(9,1,'Asia Pacific (Singapore)','Asie-Pacifique','Singapour','103.7','1.4'),</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,1,'Asia Pacific (Singapore)',21,'103.7','1.4'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1178,18 +1519,22 @@
       <c r="F11" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11">
+        <f>VLOOKUP(F11,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H11" s="1">
         <v>151</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="1">
         <v>-34</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" si="0"/>
-        <v>(10,1,'Asia Pacific (Sydney)','Asie-Pacifique','Australie','151','-34'),</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,1,'Asia Pacific (Sydney)',3,'151','-34'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1208,18 +1553,22 @@
       <c r="F12" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12">
+        <f>VLOOKUP(F12,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H12" s="1">
         <v>140</v>
       </c>
-      <c r="H12" s="6">
+      <c r="I12" s="1">
         <v>36</v>
       </c>
-      <c r="J12" t="str">
-        <f t="shared" si="0"/>
-        <v>(11,1,'Asia Pacific (Tokyo)','Asie-Pacifique','Japon','140','36'),</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,1,'Asia Pacific (Tokyo)',18,'140','36'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1238,18 +1587,22 @@
       <c r="F13" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13">
+        <f>VLOOKUP(F13,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H13" s="1">
         <v>-99</v>
       </c>
-      <c r="H13" s="6">
+      <c r="I13" s="1">
         <v>52</v>
       </c>
-      <c r="J13" t="str">
-        <f t="shared" si="0"/>
-        <v>(12,1,'Canada (Central)','Amérique du Nord','Canada','-99','52'),</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,1,'Canada (Central)',7,'-99','52'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1268,18 +1621,22 @@
       <c r="F14" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14">
+        <f>VLOOKUP(F14,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
         <v>9</v>
       </c>
-      <c r="H14" s="6">
+      <c r="I14" s="1">
         <v>50</v>
       </c>
-      <c r="J14" t="str">
-        <f t="shared" si="0"/>
-        <v>(13,1,'Europe (Frankfurt)','Europe','Allemagne','9','50'),</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="K14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,1,'Europe (Frankfurt)',2,'9','50'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1298,18 +1655,22 @@
       <c r="F15" t="s">
         <v>38</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15">
+        <f>VLOOKUP(F15,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="H15" s="1">
         <v>-7</v>
       </c>
-      <c r="H15" s="6">
+      <c r="I15" s="1">
         <v>53</v>
       </c>
-      <c r="J15" t="str">
-        <f t="shared" si="0"/>
-        <v>(14,1,'Europe (Ireland)','Europe','Irlande','-7','53'),</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="K15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,1,'Europe (Ireland)',17,'-7','53'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1328,18 +1689,22 @@
       <c r="F16" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16">
+        <f>VLOOKUP(F16,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="H16" s="1">
         <v>-0.4</v>
       </c>
-      <c r="H16" s="6">
+      <c r="I16" s="1">
         <v>51</v>
       </c>
-      <c r="J16" t="str">
-        <f t="shared" si="0"/>
-        <v>(15,1,'Europe (London)','Europe','Grande-Bretagne','-0.4','51'),</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+      <c r="K16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,1,'Europe (London)',14,'-0.4','51'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1358,18 +1723,22 @@
       <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="6">
-        <v>3</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G17">
+        <f>VLOOKUP(F17,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="H17" s="1">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1">
         <v>49</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" si="0"/>
-        <v>(16,1,'Europe (Paris)','Europe','France','3','49'),</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+      <c r="K17" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,1,'Europe (Paris)',13,'3','49'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1388,18 +1757,22 @@
       <c r="F18" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18">
+        <f>VLOOKUP(F18,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="H18" s="1">
         <v>18</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="1">
         <v>60</v>
       </c>
-      <c r="J18" t="str">
-        <f t="shared" si="0"/>
-        <v>(17,1,'Europe (Stockholm)','Europe','Suède','18','60'),</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+      <c r="K18" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,1,'Europe (Stockholm)',22,'18','60'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1418,18 +1791,22 @@
       <c r="F19" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19">
+        <f>VLOOKUP(F19,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="H19" s="1">
         <v>50.5</v>
       </c>
-      <c r="H19" s="6">
+      <c r="I19" s="1">
         <v>25.9</v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" si="0"/>
-        <v>(18,1,'Middle East (Bahrain)','Asie-Pacifique','Bahrain','50.5','25.9'),</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
+      <c r="K19" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,1,'Middle East (Bahrain)',4,'50.5','25.9'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1448,18 +1825,22 @@
       <c r="F20" t="s">
         <v>68</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20">
+        <f>VLOOKUP(F20,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="H20" s="1">
         <v>-46</v>
       </c>
-      <c r="H20" s="6">
+      <c r="I20" s="1">
         <v>-23</v>
       </c>
-      <c r="J20" t="str">
-        <f t="shared" si="0"/>
-        <v>(19,1,'South America (São Paulo)','Amérique du Sud','Brésil','-46','-23'),</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
+      <c r="K20" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,1,'South America (São Paulo)',6,'-46','-23'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1478,18 +1859,22 @@
       <c r="F21" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21">
+        <f>VLOOKUP(F21,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H21" s="1">
         <v>-66</v>
       </c>
-      <c r="H21" s="6">
+      <c r="I21" s="1">
         <v>46</v>
       </c>
-      <c r="J21" t="str">
-        <f t="shared" si="0"/>
-        <v>(20,2,'NORTHAMERICA-NORTHEAST1','Amérique du Nord','Canada','-66','46'),</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
+      <c r="K21" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,2,'NORTHAMERICA-NORTHEAST1',7,'-66','46'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>67</v>
       </c>
@@ -1508,18 +1893,22 @@
       <c r="F22" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22">
+        <f>VLOOKUP(F22,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H22" s="1">
         <v>-97</v>
       </c>
-      <c r="H22" s="6">
+      <c r="I22" s="1">
         <v>42</v>
       </c>
-      <c r="J22" t="str">
-        <f t="shared" si="0"/>
-        <v>(21,2,'US-CENTRAL1','Amérique du Nord','Etats-Unis','-97','42'),</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
+      <c r="K22" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,2,'US-CENTRAL1',11,'-97','42'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -1538,18 +1927,22 @@
       <c r="F23" t="s">
         <v>30</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23">
+        <f>VLOOKUP(F23,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H23" s="1">
         <v>-74</v>
       </c>
-      <c r="H23" s="6">
+      <c r="I23" s="1">
         <v>42</v>
       </c>
-      <c r="J23" t="str">
-        <f t="shared" si="0"/>
-        <v>(22,2,'US-EAST1','Amérique du Nord','Etats-Unis','-74','42'),</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+      <c r="K23" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,2,'US-EAST1',11,'-74','42'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>67</v>
       </c>
@@ -1568,18 +1961,22 @@
       <c r="F24" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24">
+        <f>VLOOKUP(F24,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H24" s="1">
         <v>-77</v>
       </c>
-      <c r="H24" s="6">
+      <c r="I24" s="1">
         <v>40</v>
       </c>
-      <c r="J24" t="str">
-        <f t="shared" si="0"/>
-        <v>(23,2,'US-EAST4','Amérique du Nord','Etats-Unis','-77','40'),</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10">
+      <c r="K24" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,2,'US-EAST4',11,'-77','40'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1598,18 +1995,22 @@
       <c r="F25" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25">
+        <f>VLOOKUP(F25,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H25" s="1">
         <v>-122</v>
       </c>
-      <c r="H25" s="6">
+      <c r="I25" s="1">
         <v>41</v>
       </c>
-      <c r="J25" t="str">
-        <f t="shared" si="0"/>
-        <v>(24,2,'US-WEST1','Amérique du Nord','Etats-Unis','-122','41'),</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="K25" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,2,'US-WEST1',11,'-122','41'),</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -1628,18 +2029,22 @@
       <c r="F26" t="s">
         <v>30</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26">
+        <f>VLOOKUP(F26,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H26" s="1">
         <v>-116</v>
       </c>
-      <c r="H26" s="6">
+      <c r="I26" s="1">
         <v>34</v>
       </c>
-      <c r="J26" t="str">
-        <f t="shared" si="0"/>
-        <v>(25,2,'US-WEST2','Amérique du Nord','Etats-Unis','-116','34'),</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+      <c r="K26" t="str">
+        <f t="shared" si="0"/>
+        <v>(25,2,'US-WEST2',11,'-116','34'),</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -1658,18 +2063,22 @@
       <c r="F27" t="s">
         <v>68</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27">
+        <f>VLOOKUP(F27,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="H27" s="1">
         <v>-41</v>
       </c>
-      <c r="H27" s="6">
+      <c r="I27" s="1">
         <v>-14</v>
       </c>
-      <c r="J27" t="str">
-        <f t="shared" si="0"/>
-        <v>(26,2,'SOUTHAMERICA-EAST1','Amérique du Sud','Brésil','-41','-14'),</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="K27" t="str">
+        <f t="shared" si="0"/>
+        <v>(26,2,'SOUTHAMERICA-EAST1',6,'-41','-14'),</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>67</v>
       </c>
@@ -1688,18 +2097,22 @@
       <c r="F28" t="s">
         <v>50</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28">
+        <f>VLOOKUP(F28,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="H28" s="1">
         <v>25</v>
       </c>
-      <c r="H28" s="6">
+      <c r="I28" s="1">
         <v>61</v>
       </c>
-      <c r="J28" t="str">
-        <f t="shared" si="0"/>
-        <v>(27,2,'EUROPE-NORTH1','Europe','Finlande','25','61'),</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="K28" t="str">
+        <f t="shared" si="0"/>
+        <v>(27,2,'EUROPE-NORTH1',12,'25','61'),</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -1718,18 +2131,22 @@
       <c r="F29" t="s">
         <v>52</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29">
+        <f>VLOOKUP(F29,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="H29" s="1">
         <v>4</v>
       </c>
-      <c r="H29" s="6">
+      <c r="I29" s="1">
         <v>51</v>
       </c>
-      <c r="J29" t="str">
-        <f t="shared" si="0"/>
-        <v>(28,2,'EUROPE-WEST1','Europe','Belgique','4','51'),</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="K29" t="str">
+        <f t="shared" si="0"/>
+        <v>(28,2,'EUROPE-WEST1',5,'4','51'),</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1748,18 +2165,22 @@
       <c r="F30" t="s">
         <v>39</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30">
+        <f>VLOOKUP(F30,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="H30" s="1">
         <v>-1.5</v>
       </c>
-      <c r="H30" s="6">
+      <c r="I30" s="1">
         <v>52</v>
       </c>
-      <c r="J30" t="str">
-        <f t="shared" si="0"/>
-        <v>(29,2,'EUROPE-WEST2','Europe','Grande-Bretagne','-1.5','52'),</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="K30" t="str">
+        <f t="shared" si="0"/>
+        <v>(29,2,'EUROPE-WEST2',14,'-1.5','52'),</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1778,18 +2199,22 @@
       <c r="F31" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31">
+        <f>VLOOKUP(F31,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H31" s="1">
         <v>7</v>
       </c>
-      <c r="H31" s="6">
+      <c r="I31" s="1">
         <v>50</v>
       </c>
-      <c r="J31" t="str">
-        <f t="shared" si="0"/>
-        <v>(30,2,'EUROPE-WEST3','Europe','Allemagne','7','50'),</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="K31" t="str">
+        <f t="shared" si="0"/>
+        <v>(30,2,'EUROPE-WEST3',2,'7','50'),</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>67</v>
       </c>
@@ -1808,18 +2233,22 @@
       <c r="F32" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32">
+        <f>VLOOKUP(F32,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="H32" s="1">
         <v>5.3</v>
       </c>
-      <c r="H32" s="6">
+      <c r="I32" s="1">
         <v>52</v>
       </c>
-      <c r="J32" t="str">
-        <f t="shared" si="0"/>
-        <v>(31,2,'EUROPE-WEST4','Europe','Pays-Bas','5.3','52'),</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10">
+      <c r="K32" t="str">
+        <f t="shared" si="0"/>
+        <v>(31,2,'EUROPE-WEST4',20,'5.3','52'),</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -1838,18 +2267,22 @@
       <c r="F33" t="s">
         <v>69</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33">
+        <f>VLOOKUP(F33,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="H33" s="1">
         <v>8</v>
       </c>
-      <c r="H33" s="6">
+      <c r="I33" s="1">
         <v>47</v>
       </c>
-      <c r="J33" t="str">
-        <f t="shared" si="0"/>
-        <v>(32,2,'EUROPE-WEST6','Europe','Suisse','8','47'),</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10">
+      <c r="K33" t="str">
+        <f t="shared" si="0"/>
+        <v>(32,2,'EUROPE-WEST6',23,'8','47'),</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>67</v>
       </c>
@@ -1868,18 +2301,22 @@
       <c r="F34" t="s">
         <v>59</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34">
+        <f>VLOOKUP(F34,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="H34" s="1">
         <v>121</v>
       </c>
-      <c r="H34" s="6">
+      <c r="I34" s="1">
         <v>24</v>
       </c>
-      <c r="J34" t="str">
-        <f t="shared" si="0"/>
-        <v>(33,2,'ASIA-EAST1','Asie-Pacifique','Taïwan','121','24'),</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
+      <c r="K34" t="str">
+        <f t="shared" si="0"/>
+        <v>(33,2,'ASIA-EAST1',24,'121','24'),</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -1898,18 +2335,22 @@
       <c r="F35" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35">
+        <f>VLOOKUP(F35,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="H35" s="1">
         <v>114</v>
       </c>
-      <c r="H35" s="6">
+      <c r="I35" s="1">
         <v>22</v>
       </c>
-      <c r="J35" t="str">
-        <f t="shared" si="0"/>
-        <v>(34,2,'ASIA-EAST2','Asie-Pacifique','Hong Kong','114','22'),</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10">
+      <c r="K35" t="str">
+        <f t="shared" si="0"/>
+        <v>(34,2,'ASIA-EAST2',15,'114','22'),</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -1928,18 +2369,22 @@
       <c r="F36" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36">
+        <f>VLOOKUP(F36,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H36" s="1">
         <v>139</v>
       </c>
-      <c r="H36" s="6">
+      <c r="I36" s="1">
         <v>36</v>
       </c>
-      <c r="J36" t="str">
-        <f t="shared" si="0"/>
-        <v>(35,2,'ASIA-NORTHEAST1','Asie-Pacifique','Japon','139','36'),</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10">
+      <c r="K36" t="str">
+        <f t="shared" si="0"/>
+        <v>(35,2,'ASIA-NORTHEAST1',18,'139','36'),</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1958,18 +2403,22 @@
       <c r="F37" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37">
+        <f>VLOOKUP(F37,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H37" s="1">
         <v>134</v>
       </c>
-      <c r="H37" s="6">
+      <c r="I37" s="1">
         <v>35</v>
       </c>
-      <c r="J37" t="str">
-        <f t="shared" si="0"/>
-        <v>(36,2,'ASIA-NORTHEAST2','Asie-Pacifique','Japon','134','35'),</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
+      <c r="K37" t="str">
+        <f t="shared" si="0"/>
+        <v>(36,2,'ASIA-NORTHEAST2',18,'134','35'),</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -1988,18 +2437,22 @@
       <c r="F38" t="s">
         <v>33</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38">
+        <f>VLOOKUP(F38,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="H38" s="1">
         <v>78</v>
       </c>
-      <c r="H38" s="6">
+      <c r="I38" s="1">
         <v>11</v>
       </c>
-      <c r="J38" t="str">
-        <f t="shared" si="0"/>
-        <v>(37,2,'ASIA-SOUTH1','Asie-Pacifique','Inde','78','11'),</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10">
+      <c r="K38" t="str">
+        <f t="shared" si="0"/>
+        <v>(37,2,'ASIA-SOUTH1',16,'78','11'),</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -2018,18 +2471,22 @@
       <c r="F39" t="s">
         <v>65</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39">
+        <f>VLOOKUP(F39,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="H39" s="1">
         <v>103.7</v>
       </c>
-      <c r="H39" s="6">
+      <c r="I39" s="1">
         <v>1.4</v>
       </c>
-      <c r="J39" t="str">
-        <f t="shared" si="0"/>
-        <v>(38,2,'ASIA-SOUTHEAST1','Asie-Pacifique','Singapour','103.7','1.4'),</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10">
+      <c r="K39" t="str">
+        <f t="shared" si="0"/>
+        <v>(38,2,'ASIA-SOUTHEAST1',21,'103.7','1.4'),</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -2048,18 +2505,22 @@
       <c r="F40" t="s">
         <v>36</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40">
+        <f>VLOOKUP(F40,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H40" s="1">
         <v>150</v>
       </c>
-      <c r="H40" s="6">
+      <c r="I40" s="1">
         <v>-36</v>
       </c>
-      <c r="J40" t="str">
-        <f t="shared" si="0"/>
-        <v>(39,2,'AUSTRALIA-SOUTHEAST1','Asie-Pacifique','Australie','150','-36'),</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10">
+      <c r="K40" t="str">
+        <f t="shared" si="0"/>
+        <v>(39,2,'AUSTRALIA-SOUTHEAST1',3,'150','-36'),</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -2078,18 +2539,22 @@
       <c r="F41" t="s">
         <v>24</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41">
+        <f>VLOOKUP(F41,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H41" s="1">
         <v>-73</v>
       </c>
-      <c r="H41" s="6">
+      <c r="I41" s="1">
         <v>47</v>
       </c>
-      <c r="J41" t="str">
-        <f t="shared" si="0"/>
-        <v>(40,3,'Canada East','Amérique du Nord','Canada','-73','47'),</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
+      <c r="K41" t="str">
+        <f t="shared" si="0"/>
+        <v>(40,3,'Canada East',7,'-73','47'),</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>70</v>
       </c>
@@ -2108,18 +2573,22 @@
       <c r="F42" t="s">
         <v>24</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42">
+        <f>VLOOKUP(F42,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="H42" s="1">
         <v>-113</v>
       </c>
-      <c r="H42" s="6">
+      <c r="I42" s="1">
         <v>55</v>
       </c>
-      <c r="J42" t="str">
-        <f t="shared" si="0"/>
-        <v>(41,3,'Canada Central','Amérique du Nord','Canada','-113','55'),</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
+      <c r="K42" t="str">
+        <f t="shared" si="0"/>
+        <v>(41,3,'Canada Central',7,'-113','55'),</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -2138,18 +2607,22 @@
       <c r="F43" t="s">
         <v>30</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43">
+        <f>VLOOKUP(F43,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H43" s="1">
         <v>-93.2</v>
       </c>
-      <c r="H43" s="6">
+      <c r="I43" s="1">
         <v>41.8</v>
       </c>
-      <c r="J43" t="str">
-        <f t="shared" si="0"/>
-        <v>(42,3,'US Gov Iowa','Amérique du Nord','Etats-Unis','-93.2','41.8'),</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
+      <c r="K43" t="str">
+        <f t="shared" si="0"/>
+        <v>(42,3,'US Gov Iowa',11,'-93.2','41.8'),</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>70</v>
       </c>
@@ -2168,18 +2641,22 @@
       <c r="F44" t="s">
         <v>30</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44">
+        <f>VLOOKUP(F44,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H44" s="1">
         <v>-92</v>
       </c>
-      <c r="H44" s="6">
+      <c r="I44" s="1">
         <v>37</v>
       </c>
-      <c r="J44" t="str">
-        <f t="shared" si="0"/>
-        <v>(43,3,'Central US','Amérique du Nord','Etats-Unis','-92','37'),</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10">
+      <c r="K44" t="str">
+        <f t="shared" si="0"/>
+        <v>(43,3,'Central US',11,'-92','37'),</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -2198,18 +2675,22 @@
       <c r="F45" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45">
+        <f>VLOOKUP(F45,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H45" s="1">
         <v>-93</v>
       </c>
-      <c r="H45" s="6">
+      <c r="I45" s="1">
         <v>47</v>
       </c>
-      <c r="J45" t="str">
-        <f t="shared" si="0"/>
-        <v>(44,3,'North Central US','Amérique du Nord','Etats-Unis','-93','47'),</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10">
+      <c r="K45" t="str">
+        <f t="shared" si="0"/>
+        <v>(44,3,'North Central US',11,'-93','47'),</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -2228,18 +2709,22 @@
       <c r="F46" t="s">
         <v>30</v>
       </c>
-      <c r="G46" s="6">
+      <c r="G46">
+        <f>VLOOKUP(F46,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H46" s="1">
         <v>-78</v>
       </c>
-      <c r="H46" s="6">
+      <c r="I46" s="1">
         <v>37</v>
       </c>
-      <c r="J46" t="str">
-        <f t="shared" si="0"/>
-        <v>(45,3,'US DoD East','Amérique du Nord','Etats-Unis','-78','37'),</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
+      <c r="K46" t="str">
+        <f t="shared" si="0"/>
+        <v>(45,3,'US DoD East',11,'-78','37'),</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -2258,18 +2743,22 @@
       <c r="F47" t="s">
         <v>30</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47">
+        <f>VLOOKUP(F47,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H47" s="1">
         <v>-70</v>
       </c>
-      <c r="H47" s="6">
+      <c r="I47" s="1">
         <v>44</v>
       </c>
-      <c r="J47" t="str">
-        <f t="shared" si="0"/>
-        <v>(46,3,'East US','Amérique du Nord','Etats-Unis','-70','44'),</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
+      <c r="K47" t="str">
+        <f t="shared" si="0"/>
+        <v>(46,3,'East US',11,'-70','44'),</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -2288,18 +2777,22 @@
       <c r="F48" t="s">
         <v>30</v>
       </c>
-      <c r="G48" s="6">
+      <c r="G48">
+        <f>VLOOKUP(F48,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H48" s="1">
         <v>-72</v>
       </c>
-      <c r="H48" s="6">
+      <c r="I48" s="1">
         <v>42</v>
       </c>
-      <c r="J48" t="str">
-        <f t="shared" si="0"/>
-        <v>(47,3,'East US 2','Amérique du Nord','Etats-Unis','-72','42'),</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
+      <c r="K48" t="str">
+        <f t="shared" si="0"/>
+        <v>(47,3,'East US 2',11,'-72','42'),</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>70</v>
       </c>
@@ -2318,18 +2811,22 @@
       <c r="F49" t="s">
         <v>30</v>
       </c>
-      <c r="G49" s="6">
+      <c r="G49">
+        <f>VLOOKUP(F49,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H49" s="1">
         <v>-77.8</v>
       </c>
-      <c r="H49" s="6">
+      <c r="I49" s="1">
         <v>37.700000000000003</v>
       </c>
-      <c r="J49" t="str">
-        <f t="shared" si="0"/>
-        <v>(48,3,'US Gov Virginia','Amérique du Nord','Etats-Unis','-77.8','37.7'),</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
+      <c r="K49" t="str">
+        <f t="shared" si="0"/>
+        <v>(48,3,'US Gov Virginia',11,'-77.8','37.7'),</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>70</v>
       </c>
@@ -2348,18 +2845,22 @@
       <c r="F50" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="6">
+      <c r="G50">
+        <f>VLOOKUP(F50,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H50" s="1">
         <v>-100</v>
       </c>
-      <c r="H50" s="6">
+      <c r="I50" s="1">
         <v>38</v>
       </c>
-      <c r="J50" t="str">
-        <f t="shared" si="0"/>
-        <v>(49,3,'US DoD Central','Amérique du Nord','Etats-Unis','-100','38'),</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
+      <c r="K50" t="str">
+        <f t="shared" si="0"/>
+        <v>(49,3,'US DoD Central',11,'-100','38'),</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -2378,18 +2879,22 @@
       <c r="F51" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51">
+        <f>VLOOKUP(F51,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H51" s="1">
         <v>-119</v>
       </c>
-      <c r="H51" s="6">
+      <c r="I51" s="1">
         <v>39</v>
       </c>
-      <c r="J51" t="str">
-        <f t="shared" si="0"/>
-        <v>(50,3,'West US 2','Amérique du Nord','Etats-Unis','-119','39'),</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10">
+      <c r="K51" t="str">
+        <f t="shared" si="0"/>
+        <v>(50,3,'West US 2',11,'-119','39'),</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>70</v>
       </c>
@@ -2408,18 +2913,22 @@
       <c r="F52" t="s">
         <v>30</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52">
+        <f>VLOOKUP(F52,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H52" s="1">
         <v>-109</v>
       </c>
-      <c r="H52" s="6">
+      <c r="I52" s="1">
         <v>40</v>
       </c>
-      <c r="J52" t="str">
-        <f t="shared" si="0"/>
-        <v>(51,3,'West Central US','Amérique du Nord','Etats-Unis','-109','40'),</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10">
+      <c r="K52" t="str">
+        <f t="shared" si="0"/>
+        <v>(51,3,'West Central US',11,'-109','40'),</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>70</v>
       </c>
@@ -2438,18 +2947,22 @@
       <c r="F53" t="s">
         <v>30</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53">
+        <f>VLOOKUP(F53,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H53" s="1">
         <v>-123</v>
       </c>
-      <c r="H53" s="6">
+      <c r="I53" s="1">
         <v>40</v>
       </c>
-      <c r="J53" t="str">
-        <f t="shared" si="0"/>
-        <v>(52,3,'West US','Amérique du Nord','Etats-Unis','-123','40'),</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10">
+      <c r="K53" t="str">
+        <f t="shared" si="0"/>
+        <v>(52,3,'West US',11,'-123','40'),</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -2468,18 +2981,22 @@
       <c r="F54" t="s">
         <v>30</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54">
+        <f>VLOOKUP(F54,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H54" s="1">
         <v>-111.9</v>
       </c>
-      <c r="H54" s="6">
+      <c r="I54" s="1">
         <v>33.799999999999997</v>
       </c>
-      <c r="J54" t="str">
-        <f t="shared" si="0"/>
-        <v>(53,3,'US Gov Arizona','Amérique du Nord','Etats-Unis','-111.9','33.8'),</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10">
+      <c r="K54" t="str">
+        <f t="shared" si="0"/>
+        <v>(53,3,'US Gov Arizona',11,'-111.9','33.8'),</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>70</v>
       </c>
@@ -2498,18 +3015,22 @@
       <c r="F55" t="s">
         <v>30</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55">
+        <f>VLOOKUP(F55,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H55" s="1">
         <v>-98</v>
       </c>
-      <c r="H55" s="6">
+      <c r="I55" s="1">
         <v>35</v>
       </c>
-      <c r="J55" t="str">
-        <f t="shared" si="0"/>
-        <v>(54,3,'South Central US','Amérique du Nord','Etats-Unis','-98','35'),</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10">
+      <c r="K55" t="str">
+        <f t="shared" si="0"/>
+        <v>(54,3,'South Central US',11,'-98','35'),</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2528,19 +3049,23 @@
       <c r="F56" t="s">
         <v>30</v>
       </c>
-      <c r="G56" s="6">
+      <c r="G56">
+        <f>VLOOKUP(F56,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="H56" s="1">
         <v>-97.8</v>
       </c>
-      <c r="H56" s="6">
-        <f t="shared" ref="H7:H70" ca="1" si="1">RANDBETWEEN(-50,50)</f>
-        <v>41</v>
-      </c>
-      <c r="J56" t="str">
+      <c r="I56" s="1">
+        <f t="shared" ref="I56" ca="1" si="1">RANDBETWEEN(-50,50)</f>
+        <v>45</v>
+      </c>
+      <c r="K56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(55,3,'US Gov Texas','Amérique du Nord','Etats-Unis','-97.8','41'),</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10">
+        <v>(55,3,'US Gov Texas',11,'-97.8','45'),</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>70</v>
       </c>
@@ -2559,18 +3084,22 @@
       <c r="F57" t="s">
         <v>68</v>
       </c>
-      <c r="G57" s="6">
+      <c r="G57">
+        <f>VLOOKUP(F57,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="H57" s="1">
         <v>-53</v>
       </c>
-      <c r="H57" s="6">
+      <c r="I57" s="1">
         <v>-31</v>
       </c>
-      <c r="J57" t="str">
-        <f t="shared" si="0"/>
-        <v>(56,3,'Brazil South','Amérique du Sud','Brésil','-53','-31'),</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10">
+      <c r="K57" t="str">
+        <f t="shared" si="0"/>
+        <v>(56,3,'Brazil South',6,'-53','-31'),</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -2589,18 +3118,22 @@
       <c r="F58" t="s">
         <v>102</v>
       </c>
-      <c r="G58" s="6">
+      <c r="G58">
+        <f>VLOOKUP(F58,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="H58" s="1">
         <v>6</v>
       </c>
-      <c r="H58" s="6">
+      <c r="I58" s="1">
         <v>60</v>
       </c>
-      <c r="J58" t="str">
-        <f t="shared" si="0"/>
-        <v>(57,3,'Norway West','Europe','Norvège','6','60'),</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10">
+      <c r="K58" t="str">
+        <f t="shared" si="0"/>
+        <v>(57,3,'Norway West',19,'6','60'),</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -2619,18 +3152,22 @@
       <c r="F59" t="s">
         <v>56</v>
       </c>
-      <c r="G59" s="6">
+      <c r="G59">
+        <f>VLOOKUP(F59,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="H59" s="1">
         <v>5.4</v>
       </c>
-      <c r="H59" s="6">
+      <c r="I59" s="1">
         <v>52</v>
       </c>
-      <c r="J59" t="str">
-        <f t="shared" si="0"/>
-        <v>(58,3,'West Europe','Europe','Pays-Bas','5.4','52'),</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10">
+      <c r="K59" t="str">
+        <f t="shared" si="0"/>
+        <v>(58,3,'West Europe',20,'5.4','52'),</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -2649,18 +3186,22 @@
       <c r="F60" t="s">
         <v>39</v>
       </c>
-      <c r="G60" s="6">
+      <c r="G60">
+        <f>VLOOKUP(F60,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="H60" s="1">
         <v>-1.8</v>
       </c>
-      <c r="H60" s="6">
+      <c r="I60" s="1">
         <v>51</v>
       </c>
-      <c r="J60" t="str">
-        <f t="shared" si="0"/>
-        <v>(59,3,'UK South','Europe','Grande-Bretagne','-1.8','51'),</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10">
+      <c r="K60" t="str">
+        <f t="shared" si="0"/>
+        <v>(59,3,'UK South',14,'-1.8','51'),</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -2679,18 +3220,22 @@
       <c r="F61" t="s">
         <v>38</v>
       </c>
-      <c r="G61" s="6">
+      <c r="G61">
+        <f>VLOOKUP(F61,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="H61" s="1">
         <v>-9</v>
       </c>
-      <c r="H61" s="6">
+      <c r="I61" s="1">
         <v>52</v>
       </c>
-      <c r="J61" t="str">
-        <f t="shared" si="0"/>
-        <v>(60,3,'North Europe','Europe','Irlande','-9','52'),</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
+      <c r="K61" t="str">
+        <f t="shared" si="0"/>
+        <v>(60,3,'North Europe',17,'-9','52'),</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -2709,18 +3254,22 @@
       <c r="F62" t="s">
         <v>39</v>
       </c>
-      <c r="G62" s="6">
+      <c r="G62">
+        <f>VLOOKUP(F62,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="H62" s="1">
         <v>-4</v>
       </c>
-      <c r="H62" s="6">
+      <c r="I62" s="1">
         <v>52</v>
       </c>
-      <c r="J62" t="str">
-        <f t="shared" si="0"/>
-        <v>(61,3,'UK West','Europe','Grande-Bretagne','-4','52'),</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
+      <c r="K62" t="str">
+        <f t="shared" si="0"/>
+        <v>(61,3,'UK West',14,'-4','52'),</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -2739,18 +3288,22 @@
       <c r="F63" t="s">
         <v>40</v>
       </c>
-      <c r="G63" s="6">
+      <c r="G63">
+        <f>VLOOKUP(F63,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="H63" s="1">
         <v>2</v>
       </c>
-      <c r="H63" s="6">
+      <c r="I63" s="1">
         <v>47</v>
       </c>
-      <c r="J63" t="str">
-        <f t="shared" si="0"/>
-        <v>(62,3,'France Central','Europe','France','2','47'),</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
+      <c r="K63" t="str">
+        <f t="shared" si="0"/>
+        <v>(62,3,'France Central',13,'2','47'),</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -2769,18 +3322,22 @@
       <c r="F64" t="s">
         <v>40</v>
       </c>
-      <c r="G64" s="6">
-        <v>3</v>
-      </c>
-      <c r="H64" s="6">
+      <c r="G64">
+        <f>VLOOKUP(F64,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="H64" s="1">
+        <v>3</v>
+      </c>
+      <c r="I64" s="1">
         <v>44</v>
       </c>
-      <c r="J64" t="str">
-        <f t="shared" si="0"/>
-        <v>(63,3,'France South','Europe','France','3','44'),</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="K64" t="str">
+        <f t="shared" si="0"/>
+        <v>(63,3,'France South',13,'3','44'),</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -2799,18 +3356,22 @@
       <c r="F65" t="s">
         <v>69</v>
       </c>
-      <c r="G65" s="6">
+      <c r="G65">
+        <f>VLOOKUP(F65,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="H65" s="1">
         <v>7</v>
       </c>
-      <c r="H65" s="6">
+      <c r="I65" s="1">
         <v>47</v>
       </c>
-      <c r="J65" t="str">
-        <f t="shared" si="0"/>
-        <v>(64,3,'Switzerland West','Europe','Suisse','7','47'),</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
+      <c r="K65" t="str">
+        <f t="shared" si="0"/>
+        <v>(64,3,'Switzerland West',23,'7','47'),</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>70</v>
       </c>
@@ -2829,18 +3390,22 @@
       <c r="F66" t="s">
         <v>69</v>
       </c>
-      <c r="G66" s="6">
+      <c r="G66">
+        <f>VLOOKUP(F66,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="H66" s="1">
         <v>8</v>
       </c>
-      <c r="H66" s="6">
+      <c r="I66" s="1">
         <v>47</v>
       </c>
-      <c r="J66" t="str">
-        <f t="shared" si="0"/>
-        <v>(65,3,'Switzerland North','Europe','Suisse','8','47'),</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
+      <c r="K66" t="str">
+        <f t="shared" si="0"/>
+        <v>(65,3,'Switzerland North',23,'8','47'),</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -2859,18 +3424,22 @@
       <c r="F67" t="s">
         <v>37</v>
       </c>
-      <c r="G67" s="6">
+      <c r="G67">
+        <f>VLOOKUP(F67,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H67" s="1">
         <v>11</v>
       </c>
-      <c r="H67" s="6">
+      <c r="I67" s="1">
         <v>52</v>
       </c>
-      <c r="J67" t="str">
-        <f t="shared" ref="J67:J92" si="2">CONCATENATE("(",B67,",",C67,",'",D67,"','",E67,"','",F67,"','",G67,"','",H67,"'),")</f>
-        <v>(66,3,'Germany Central','Europe','Allemagne','11','52'),</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
+      <c r="K67" t="str">
+        <f t="shared" ref="K67:K92" si="2">CONCATENATE("(",B67,",",C67,",'",D67,"',",G67,",'",H67,"','",I67,"'),")</f>
+        <v>(66,3,'Germany Central',2,'11','52'),</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>70</v>
       </c>
@@ -2889,18 +3458,22 @@
       <c r="F68" t="s">
         <v>37</v>
       </c>
-      <c r="G68" s="6">
+      <c r="G68">
+        <f>VLOOKUP(F68,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H68" s="1">
         <v>8</v>
       </c>
-      <c r="H68" s="6">
+      <c r="I68" s="1">
         <v>53</v>
       </c>
-      <c r="J68" t="str">
+      <c r="K68" t="str">
         <f t="shared" si="2"/>
-        <v>(67,3,'Germany Northeast','Europe','Allemagne','8','53'),</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
+        <v>(67,3,'Germany Northeast',2,'8','53'),</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -2919,18 +3492,22 @@
       <c r="F69" t="s">
         <v>37</v>
       </c>
-      <c r="G69" s="6">
+      <c r="G69">
+        <f>VLOOKUP(F69,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H69" s="1">
         <v>11</v>
       </c>
-      <c r="H69" s="6">
+      <c r="I69" s="1">
         <v>54</v>
       </c>
-      <c r="J69" t="str">
+      <c r="K69" t="str">
         <f t="shared" si="2"/>
-        <v>(68,3,'Germany North','Europe','Allemagne','11','54'),</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
+        <v>(68,3,'Germany North',2,'11','54'),</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -2949,18 +3526,22 @@
       <c r="F70" t="s">
         <v>37</v>
       </c>
-      <c r="G70" s="6">
+      <c r="G70">
+        <f>VLOOKUP(F70,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="H70" s="1">
         <v>9</v>
       </c>
-      <c r="H70" s="6">
+      <c r="I70" s="1">
         <v>49</v>
       </c>
-      <c r="J70" t="str">
+      <c r="K70" t="str">
         <f t="shared" si="2"/>
-        <v>(69,3,'Germany West Central','Europe','Allemagne','9','49'),</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
+        <v>(69,3,'Germany West Central',2,'9','49'),</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2979,18 +3560,22 @@
       <c r="F71" t="s">
         <v>102</v>
       </c>
-      <c r="G71" s="6">
+      <c r="G71">
+        <f>VLOOKUP(F71,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="H71" s="1">
         <v>11</v>
       </c>
-      <c r="H71" s="6">
+      <c r="I71" s="1">
         <v>60</v>
       </c>
-      <c r="J71" t="str">
+      <c r="K71" t="str">
         <f t="shared" si="2"/>
-        <v>(70,3,'Norway East','Europe','Norvège','11','60'),</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
+        <v>(70,3,'Norway East',19,'11','60'),</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>70</v>
       </c>
@@ -3009,18 +3594,22 @@
       <c r="F72" t="s">
         <v>106</v>
       </c>
-      <c r="G72" s="6">
+      <c r="G72">
+        <f>VLOOKUP(F72,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H72" s="1">
         <v>19</v>
       </c>
-      <c r="H72" s="6">
+      <c r="I72" s="1">
         <v>-33</v>
       </c>
-      <c r="J72" t="str">
+      <c r="K72" t="str">
         <f t="shared" si="2"/>
-        <v>(71,3,'South Africa West','Afrique','Afrique du Sud','19','-33'),</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
+        <v>(71,3,'South Africa West',1,'19','-33'),</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -3039,18 +3628,22 @@
       <c r="F73" t="s">
         <v>106</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G73">
+        <f>VLOOKUP(F73,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="H73" s="1">
         <v>28</v>
       </c>
-      <c r="H73" s="6">
+      <c r="I73" s="1">
         <v>-26</v>
       </c>
-      <c r="J73" t="str">
+      <c r="K73" t="str">
         <f t="shared" si="2"/>
-        <v>(72,3,'South Africa North','Afrique','Afrique du Sud','28','-26'),</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
+        <v>(72,3,'South Africa North',1,'28','-26'),</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -3069,18 +3662,22 @@
       <c r="F74" t="s">
         <v>126</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G74">
+        <f>VLOOKUP(F74,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="H74" s="1">
         <v>55</v>
       </c>
-      <c r="H74" s="6">
+      <c r="I74" s="1">
         <v>24</v>
       </c>
-      <c r="J74" t="str">
+      <c r="K74" t="str">
         <f t="shared" si="2"/>
-        <v>(73,3,'UAE Central','Asie-Pacifique','Emirats Arabes Unis','55','24'),</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
+        <v>(73,3,'UAE Central',10,'55','24'),</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>70</v>
       </c>
@@ -3099,18 +3696,22 @@
       <c r="F75" t="s">
         <v>126</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G75">
+        <f>VLOOKUP(F75,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="H75" s="1">
         <v>56</v>
       </c>
-      <c r="H75" s="6">
+      <c r="I75" s="1">
         <v>25</v>
       </c>
-      <c r="J75" t="str">
+      <c r="K75" t="str">
         <f t="shared" si="2"/>
-        <v>(74,3,'UAE North','Asie-Pacifique','Emirats Arabes Unis','56','25'),</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
+        <v>(74,3,'UAE North',10,'56','25'),</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>70</v>
       </c>
@@ -3129,18 +3730,22 @@
       <c r="F76" t="s">
         <v>33</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76">
+        <f>VLOOKUP(F76,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="H76" s="1">
         <v>74</v>
       </c>
-      <c r="H76" s="6">
+      <c r="I76" s="1">
         <v>17</v>
       </c>
-      <c r="J76" t="str">
+      <c r="K76" t="str">
         <f t="shared" si="2"/>
-        <v>(75,3,'West India','Asie-Pacifique','Inde','74','17'),</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
+        <v>(75,3,'West India',16,'74','17'),</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>70</v>
       </c>
@@ -3159,18 +3764,22 @@
       <c r="F77" t="s">
         <v>33</v>
       </c>
-      <c r="G77" s="6">
+      <c r="G77">
+        <f>VLOOKUP(F77,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="H77" s="1">
         <v>78</v>
       </c>
-      <c r="H77" s="6">
+      <c r="I77" s="1">
         <v>20</v>
       </c>
-      <c r="J77" t="str">
+      <c r="K77" t="str">
         <f t="shared" si="2"/>
-        <v>(76,3,'Central India','Asie-Pacifique','Inde','78','20'),</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
+        <v>(76,3,'Central India',16,'78','20'),</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>70</v>
       </c>
@@ -3189,18 +3798,22 @@
       <c r="F78" t="s">
         <v>33</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78">
+        <f>VLOOKUP(F78,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="H78" s="1">
         <v>77</v>
       </c>
-      <c r="H78" s="6">
+      <c r="I78" s="1">
         <v>11</v>
       </c>
-      <c r="J78" t="str">
+      <c r="K78" t="str">
         <f t="shared" si="2"/>
-        <v>(77,3,'South India','Asie-Pacifique','Inde','77','11'),</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
+        <v>(77,3,'South India',16,'77','11'),</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>70</v>
       </c>
@@ -3219,18 +3832,22 @@
       <c r="F79" t="s">
         <v>65</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79">
+        <f>VLOOKUP(F79,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="H79" s="1">
         <v>103.7</v>
       </c>
-      <c r="H79" s="6">
+      <c r="I79" s="1">
         <v>1.4</v>
       </c>
-      <c r="J79" t="str">
+      <c r="K79" t="str">
         <f t="shared" si="2"/>
-        <v>(78,3,'Southeast Asia','Asie-Pacifique','Singapour','103.7','1.4'),</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10">
+        <v>(78,3,'Southeast Asia',21,'103.7','1.4'),</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>70</v>
       </c>
@@ -3249,18 +3866,22 @@
       <c r="F80" t="s">
         <v>127</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80">
+        <f>VLOOKUP(F80,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="H80" s="1">
         <v>115</v>
       </c>
-      <c r="H80" s="6">
+      <c r="I80" s="1">
         <v>39</v>
       </c>
-      <c r="J80" t="str">
+      <c r="K80" t="str">
         <f t="shared" si="2"/>
-        <v>(79,3,'China North','Asie-Pacifique','Chine','115','39'),</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10">
+        <v>(79,3,'China North',8,'115','39'),</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>70</v>
       </c>
@@ -3279,18 +3900,22 @@
       <c r="F81" t="s">
         <v>127</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G81">
+        <f>VLOOKUP(F81,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="H81" s="1">
         <v>118</v>
       </c>
-      <c r="H81" s="6">
+      <c r="I81" s="1">
         <v>37</v>
       </c>
-      <c r="J81" t="str">
+      <c r="K81" t="str">
         <f t="shared" si="2"/>
-        <v>(80,3,'China North 2','Asie-Pacifique','Chine','118','37'),</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10">
+        <v>(80,3,'China North 2',8,'118','37'),</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>70</v>
       </c>
@@ -3309,18 +3934,22 @@
       <c r="F82" t="s">
         <v>35</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82">
+        <f>VLOOKUP(F82,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="H82" s="1">
         <v>128</v>
       </c>
-      <c r="H82" s="6">
+      <c r="I82" s="1">
         <v>36</v>
       </c>
-      <c r="J82" t="str">
+      <c r="K82" t="str">
         <f t="shared" si="2"/>
-        <v>(81,3,'Korea Central','Asie-Pacifique','Corée du Sud','128','36'),</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10">
+        <v>(81,3,'Korea Central',9,'128','36'),</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>70</v>
       </c>
@@ -3339,18 +3968,22 @@
       <c r="F83" t="s">
         <v>35</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83">
+        <f>VLOOKUP(F83,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="H83" s="1">
         <v>127</v>
       </c>
-      <c r="H83" s="6">
+      <c r="I83" s="1">
         <v>35</v>
       </c>
-      <c r="J83" t="str">
+      <c r="K83" t="str">
         <f t="shared" si="2"/>
-        <v>(82,3,'Korea South','Asie-Pacifique','Corée du Sud','127','35'),</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10">
+        <v>(82,3,'Korea South',9,'127','35'),</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>70</v>
       </c>
@@ -3369,18 +4002,22 @@
       <c r="F84" t="s">
         <v>127</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84">
+        <f>VLOOKUP(F84,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="H84" s="1">
         <v>121</v>
       </c>
-      <c r="H84" s="6">
+      <c r="I84" s="1">
         <v>30</v>
       </c>
-      <c r="J84" t="str">
+      <c r="K84" t="str">
         <f t="shared" si="2"/>
-        <v>(83,3,'China East','Asie-Pacifique','Chine','121','30'),</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10">
+        <v>(83,3,'China East',8,'121','30'),</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>70</v>
       </c>
@@ -3399,18 +4036,22 @@
       <c r="F85" t="s">
         <v>127</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G85">
+        <f>VLOOKUP(F85,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="H85" s="1">
         <v>120</v>
       </c>
-      <c r="H85" s="6">
+      <c r="I85" s="1">
         <v>28</v>
       </c>
-      <c r="J85" t="str">
+      <c r="K85" t="str">
         <f t="shared" si="2"/>
-        <v>(84,3,'China East 2','Asie-Pacifique','Chine','120','28'),</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10">
+        <v>(84,3,'China East 2',8,'120','28'),</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>70</v>
       </c>
@@ -3429,18 +4070,22 @@
       <c r="F86" t="s">
         <v>127</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G86">
+        <f>VLOOKUP(F86,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="H86" s="1">
         <v>115</v>
       </c>
-      <c r="H86" s="6">
+      <c r="I86" s="1">
         <v>23</v>
       </c>
-      <c r="J86" t="str">
+      <c r="K86" t="str">
         <f t="shared" si="2"/>
-        <v>(85,3,'East Asia','Asie-Pacifique','Chine','115','23'),</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10">
+        <v>(85,3,'East Asia',8,'115','23'),</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>70</v>
       </c>
@@ -3459,18 +4104,22 @@
       <c r="F87" t="s">
         <v>34</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87">
+        <f>VLOOKUP(F87,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H87" s="1">
         <v>140</v>
       </c>
-      <c r="H87" s="6">
+      <c r="I87" s="1">
         <v>37</v>
       </c>
-      <c r="J87" t="str">
+      <c r="K87" t="str">
         <f t="shared" si="2"/>
-        <v>(86,3,'Japan East','Asie-Pacifique','Japon','140','37'),</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10">
+        <v>(86,3,'Japan East',18,'140','37'),</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>70</v>
       </c>
@@ -3489,18 +4138,22 @@
       <c r="F88" t="s">
         <v>34</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G88">
+        <f>VLOOKUP(F88,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="H88" s="1">
         <v>131</v>
       </c>
-      <c r="H88" s="6">
+      <c r="I88" s="1">
         <v>33</v>
       </c>
-      <c r="J88" t="str">
+      <c r="K88" t="str">
         <f t="shared" si="2"/>
-        <v>(87,3,'Japan West','Asie-Pacifique','Japon','131','33'),</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10">
+        <v>(87,3,'Japan West',18,'131','33'),</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>70</v>
       </c>
@@ -3519,18 +4172,22 @@
       <c r="F89" t="s">
         <v>36</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G89">
+        <f>VLOOKUP(F89,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H89" s="1">
         <v>151</v>
       </c>
-      <c r="H89" s="6">
+      <c r="I89" s="1">
         <v>-31</v>
       </c>
-      <c r="J89" t="str">
+      <c r="K89" t="str">
         <f t="shared" si="2"/>
-        <v>(88,3,'Australia East','Asie-Pacifique','Australie','151','-31'),</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10">
+        <v>(88,3,'Australia East',3,'151','-31'),</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>70</v>
       </c>
@@ -3549,18 +4206,22 @@
       <c r="F90" t="s">
         <v>36</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90">
+        <f>VLOOKUP(F90,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H90" s="1">
         <v>148</v>
       </c>
-      <c r="H90" s="6">
+      <c r="I90" s="1">
         <v>-37</v>
       </c>
-      <c r="J90" t="str">
+      <c r="K90" t="str">
         <f t="shared" si="2"/>
-        <v>(89,3,'Australia Southeast','Asie-Pacifique','Australie','148','-37'),</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10">
+        <v>(89,3,'Australia Southeast',3,'148','-37'),</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>70</v>
       </c>
@@ -3579,18 +4240,22 @@
       <c r="F91" t="s">
         <v>36</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G91">
+        <f>VLOOKUP(F91,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H91" s="1">
         <v>132</v>
       </c>
-      <c r="H91" s="6">
+      <c r="I91" s="1">
         <v>-29</v>
       </c>
-      <c r="J91" t="str">
+      <c r="K91" t="str">
         <f t="shared" si="2"/>
-        <v>(90,3,'Australia Central','Asie-Pacifique','Australie','132','-29'),</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10">
+        <v>(90,3,'Australia Central',3,'132','-29'),</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>70</v>
       </c>
@@ -3609,144 +4274,646 @@
       <c r="F92" t="s">
         <v>36</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G92">
+        <f>VLOOKUP(F92,countries!$A$2:$B$25,2,FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="H92" s="1">
         <v>133</v>
       </c>
-      <c r="H92" s="6">
+      <c r="I92" s="1">
         <v>-24</v>
       </c>
-      <c r="J92" t="str">
+      <c r="K92" t="str">
         <f t="shared" si="2"/>
-        <v>(91,3,'Australia Central 2','Asie-Pacifique','Australie','133','-24'),</v>
+        <v>(91,3,'Australia Central 2',3,'133','-24'),</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J92" xr:uid="{B13B48CD-DB70-48DF-9873-24BF54116718}"/>
+  <autoFilter ref="A1:K92" xr:uid="{B13B48CD-DB70-48DF-9873-24BF54116718}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE2D952-D49D-4F87-9861-AA9CC2EDC2B7}">
-  <dimension ref="A1:C21"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCC7AF2-63E8-4903-A10A-E69C9361DEC6}">
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C18:C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickBot="1">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="2"/>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="15" thickBot="1">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" ht="15" thickBot="1">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="15" thickBot="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" ht="15" thickBot="1">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" ht="15" thickBot="1">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" ht="15" thickBot="1">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" thickBot="1">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" thickBot="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" thickBot="1">
-      <c r="A17" s="2"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" thickBot="1">
-      <c r="A18" s="2"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" thickBot="1">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" ht="15" thickBot="1">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="E2">
+        <v>4.96</v>
+      </c>
+      <c r="F2">
+        <v>0.70499999999999996</v>
+      </c>
+      <c r="G2" t="str">
+        <f>CONCATENATE("(",B2,",'",A2,"','",C2,"','",D2,"','",E2,"','",F2,"'),")</f>
+        <v>(1,'Afrique du Sud','Afrique','71.1','4.96','0.705'),</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>24.7</v>
+      </c>
+      <c r="E3">
+        <v>8.39</v>
+      </c>
+      <c r="F3">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G25" si="0">CONCATENATE("(",B3,",'",A3,"','",C3,"','",D3,"','",E3,"','",F3,"'),")</f>
+        <v>(2,'Allemagne','Europe','24.7','8.39','0.939'),</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>19.7</v>
+      </c>
+      <c r="E4">
+        <v>8.24</v>
+      </c>
+      <c r="F4">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>(3,'Australie','Europe','19.7','8.24','0.938'),</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>63.8</v>
+      </c>
+      <c r="E5">
+        <v>7.6</v>
+      </c>
+      <c r="F5">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>(4,'Bahrain','Asie-Pacifique','63.8','7.6','0.838'),</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>28.6</v>
+      </c>
+      <c r="E6">
+        <v>7.81</v>
+      </c>
+      <c r="F6">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>(5,'Belgique','Europe','28.6','7.81','0.919'),</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7">
+        <v>71.8</v>
+      </c>
+      <c r="E7">
+        <v>6.12</v>
+      </c>
+      <c r="F7">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>(6,'Brésil','Amérique du Sud','71.8','6.12','0.761'),</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>7.93</v>
+      </c>
+      <c r="F8">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>(7,'Canada','Amérique du Nord','20','7.93','0.922'),</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="E9">
+        <v>7.83</v>
+      </c>
+      <c r="F9">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>(8,'Chine','Asie-Pacifique','71.1','7.83','0.758'),</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="E10">
+        <v>8.85</v>
+      </c>
+      <c r="F10">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>(9,'Corée du Sud','Asie-Pacifique','33.7','8.85','0.906'),</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>40.1</v>
+      </c>
+      <c r="E11">
+        <v>7.21</v>
+      </c>
+      <c r="F11">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>(10,'Emirats Arabes Unis','Asie-Pacifique','40.1','7.21','0.866'),</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>8.18</v>
+      </c>
+      <c r="F12">
+        <v>0.92</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>(11,'Etats-Unis','Amérique du Nord','38','8.18','0.92'),</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E13">
+        <v>7.88</v>
+      </c>
+      <c r="F13">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>(12,'Finlande','Europe','16.9','7.88','0.925'),</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>8.24</v>
+      </c>
+      <c r="F14">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>(13,'France','Europe','32','8.24','0.891'),</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="E15">
+        <v>8.65</v>
+      </c>
+      <c r="F15">
+        <v>0.92</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>(14,'Grande-Bretagne','Europe','36.7','8.65','0.92'),</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>52.4</v>
+      </c>
+      <c r="E16">
+        <v>8.61</v>
+      </c>
+      <c r="F16">
+        <v>0.93899999999999995</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>(15,'Hong Kong','Asie-Pacifique','52.4','8.61','0.939'),</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="E17">
+        <v>3.03</v>
+      </c>
+      <c r="F17">
+        <v>0.64700000000000002</v>
+      </c>
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>(16,'Inde','Asie-Pacifique','74.4','3.03','0.647'),</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18">
+        <v>20.6</v>
+      </c>
+      <c r="E18">
+        <v>8.02</v>
+      </c>
+      <c r="F18">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>(17,'Irlande','Europe','20.6','8.02','0.942'),</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="E19">
+        <v>8.43</v>
+      </c>
+      <c r="F19">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>(18,'Japon','Asie-Pacifique','34.3','8.43','0.915'),</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>18</v>
+      </c>
+      <c r="E20">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="F20">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>(19,'Norvège','Europe','18','8.45','0.954'),</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>24.8</v>
+      </c>
+      <c r="E21">
+        <v>8.4</v>
+      </c>
+      <c r="F21">
+        <v>0.93300000000000005</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>(20,'Pays-Bas','Europe','24.8','8.4','0.933'),</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>28.1</v>
+      </c>
+      <c r="E22">
+        <v>7.85</v>
+      </c>
+      <c r="F22">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>(21,'Singapour','Asie-Pacifique','28.1','7.85','0.935'),</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <v>20.3</v>
+      </c>
+      <c r="E23">
+        <v>8.41</v>
+      </c>
+      <c r="F23">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>(22,'Suède','Europe','20.3','8.41','0.937'),</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <v>18.7</v>
+      </c>
+      <c r="E24">
+        <v>8.66</v>
+      </c>
+      <c r="F24">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>(23,'Suisse','Europe','18.7','8.66','0.946'),</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25">
+        <v>61.1</v>
+      </c>
+      <c r="E25">
+        <v>7.8</v>
+      </c>
+      <c r="F25">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>(24,'Taïwan','Asie-Pacifique','61.1','7.8','0.923'),</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A92">
+    <sortCondition ref="A2:A92"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create doc storage page, link to marker
</commit_message>
<xml_diff>
--- a/data/db/data providers.xlsx
+++ b/data/db/data providers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAFF2AF-3B1D-45BD-AE03-FE0C2B7623B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C97131-F9CE-42CB-B293-E82FE8B6E0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
   </bookViews>
@@ -4301,7 +4301,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G25"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add sustainability score for storage locations
</commit_message>
<xml_diff>
--- a/data/db/data providers.xlsx
+++ b/data/db/data providers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HabibElHourani\Desktop\tools\test2\longevity\data\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00C97131-F9CE-42CB-B293-E82FE8B6E0C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4C8A58-E080-4584-B428-34E31ECAA196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{29C7688C-5A64-4828-B5DB-9FC14559E063}"/>
   </bookViews>
   <sheets>
     <sheet name="data providers" sheetId="3" r:id="rId1"/>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87765F3-A5A8-4725-B7FA-B36A7F3DBCF9}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13:J15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3058,11 +3058,11 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" ref="I56" ca="1" si="1">RANDBETWEEN(-50,50)</f>
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="K56" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>(55,3,'US Gov Texas',11,'-97.8','45'),</v>
+        <v>(55,3,'US Gov Texas',11,'-97.8','30'),</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
@@ -4300,7 +4300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FCC7AF2-63E8-4903-A10A-E69C9361DEC6}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>

</xml_diff>